<commit_message>
cierre 10 Oct 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #09 SEPTIEMBRE 2022/BALANCE   HERRADURA SEPTIEMBRE      2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #09 SEPTIEMBRE 2022/BALANCE   HERRADURA SEPTIEMBRE      2022.xlsx
@@ -572,7 +572,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="471">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -1995,6 +1995,9 @@
   </si>
   <si>
     <t>Longaniza-chorizo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMINA # 39  </t>
   </si>
 </sst>
 </file>
@@ -3904,6 +3907,13 @@
     <xf numFmtId="44" fontId="2" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="16" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="19" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="7" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4030,13 +4040,6 @@
     <xf numFmtId="166" fontId="12" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="19" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="7" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -8191,23 +8194,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="314"/>
-      <c r="C1" s="316" t="s">
+      <c r="B1" s="317"/>
+      <c r="C1" s="319" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="317"/>
-      <c r="E1" s="317"/>
-      <c r="F1" s="317"/>
-      <c r="G1" s="317"/>
-      <c r="H1" s="317"/>
-      <c r="I1" s="317"/>
-      <c r="J1" s="317"/>
-      <c r="K1" s="317"/>
-      <c r="L1" s="317"/>
-      <c r="M1" s="317"/>
+      <c r="D1" s="320"/>
+      <c r="E1" s="320"/>
+      <c r="F1" s="320"/>
+      <c r="G1" s="320"/>
+      <c r="H1" s="320"/>
+      <c r="I1" s="320"/>
+      <c r="J1" s="320"/>
+      <c r="K1" s="320"/>
+      <c r="L1" s="320"/>
+      <c r="M1" s="320"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="315"/>
+      <c r="B2" s="318"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -8217,21 +8220,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="318" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="319"/>
+      <c r="B3" s="321" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="322"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="320" t="s">
+      <c r="H3" s="323" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="320"/>
+      <c r="I3" s="323"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="325" t="s">
+      <c r="R3" s="328" t="s">
         <v>38</v>
       </c>
     </row>
@@ -8246,14 +8249,14 @@
       <c r="D4" s="16">
         <v>44563</v>
       </c>
-      <c r="E4" s="321" t="s">
+      <c r="E4" s="324" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="322"/>
-      <c r="H4" s="323" t="s">
+      <c r="F4" s="325"/>
+      <c r="H4" s="326" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="324"/>
+      <c r="I4" s="327"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -8263,11 +8266,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="332" t="s">
+      <c r="P4" s="335" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="333"/>
-      <c r="R4" s="326"/>
+      <c r="Q4" s="336"/>
+      <c r="R4" s="329"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -9722,11 +9725,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="87"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="334">
+      <c r="M40" s="337">
         <f>SUM(M5:M39)</f>
         <v>1527030</v>
       </c>
-      <c r="N40" s="336">
+      <c r="N40" s="339">
         <f>SUM(N5:N39)</f>
         <v>50013</v>
       </c>
@@ -9751,8 +9754,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="74"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="335"/>
-      <c r="N41" s="337"/>
+      <c r="M41" s="338"/>
+      <c r="N41" s="340"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -9959,29 +9962,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="338" t="s">
+      <c r="H53" s="341" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="339"/>
+      <c r="I53" s="342"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="340">
+      <c r="K53" s="343">
         <f>I51+L51</f>
         <v>50143.28</v>
       </c>
-      <c r="L53" s="341"/>
-      <c r="M53" s="342">
+      <c r="L53" s="344"/>
+      <c r="M53" s="345">
         <f>N40+M40</f>
         <v>1577043</v>
       </c>
-      <c r="N53" s="343"/>
+      <c r="N53" s="346"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="344" t="s">
+      <c r="D54" s="347" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="344"/>
+      <c r="E54" s="347"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>1561421.72</v>
@@ -9992,22 +9995,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="345" t="s">
+      <c r="D55" s="348" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="345"/>
+      <c r="E55" s="348"/>
       <c r="F55" s="111">
         <v>-1419082.77</v>
       </c>
-      <c r="I55" s="346" t="s">
+      <c r="I55" s="349" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="347"/>
-      <c r="K55" s="348">
+      <c r="J55" s="350"/>
+      <c r="K55" s="351">
         <f>F57+F58+F59</f>
         <v>296963.46999999997</v>
       </c>
-      <c r="L55" s="349"/>
+      <c r="L55" s="352"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -10038,11 +10041,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="350">
+      <c r="K57" s="353">
         <f>-C4</f>
         <v>-221059.7</v>
       </c>
-      <c r="L57" s="351"/>
+      <c r="L57" s="354"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -10059,22 +10062,22 @@
       <c r="C59" s="128">
         <v>44591</v>
       </c>
-      <c r="D59" s="327" t="s">
+      <c r="D59" s="330" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="328"/>
+      <c r="E59" s="331"/>
       <c r="F59" s="129">
         <v>154314.51999999999</v>
       </c>
-      <c r="I59" s="329" t="s">
+      <c r="I59" s="332" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="330"/>
-      <c r="K59" s="331">
+      <c r="J59" s="333"/>
+      <c r="K59" s="334">
         <f>K55+K57</f>
         <v>75903.76999999996</v>
       </c>
-      <c r="L59" s="331"/>
+      <c r="L59" s="334"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -11672,23 +11675,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="314"/>
-      <c r="C1" s="316" t="s">
+      <c r="B1" s="317"/>
+      <c r="C1" s="319" t="s">
         <v>326</v>
       </c>
-      <c r="D1" s="317"/>
-      <c r="E1" s="317"/>
-      <c r="F1" s="317"/>
-      <c r="G1" s="317"/>
-      <c r="H1" s="317"/>
-      <c r="I1" s="317"/>
-      <c r="J1" s="317"/>
-      <c r="K1" s="317"/>
-      <c r="L1" s="317"/>
-      <c r="M1" s="317"/>
+      <c r="D1" s="320"/>
+      <c r="E1" s="320"/>
+      <c r="F1" s="320"/>
+      <c r="G1" s="320"/>
+      <c r="H1" s="320"/>
+      <c r="I1" s="320"/>
+      <c r="J1" s="320"/>
+      <c r="K1" s="320"/>
+      <c r="L1" s="320"/>
+      <c r="M1" s="320"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="315"/>
+      <c r="B2" s="318"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -11698,21 +11701,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="318" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="319"/>
+      <c r="B3" s="321" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="322"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="320" t="s">
+      <c r="H3" s="323" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="320"/>
+      <c r="I3" s="323"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="325" t="s">
+      <c r="R3" s="328" t="s">
         <v>38</v>
       </c>
     </row>
@@ -11727,14 +11730,14 @@
       <c r="D4" s="16">
         <v>44710</v>
       </c>
-      <c r="E4" s="321" t="s">
+      <c r="E4" s="324" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="322"/>
-      <c r="H4" s="323" t="s">
+      <c r="F4" s="325"/>
+      <c r="H4" s="326" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="324"/>
+      <c r="I4" s="327"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -11744,11 +11747,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="332" t="s">
+      <c r="P4" s="335" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="333"/>
-      <c r="R4" s="326"/>
+      <c r="Q4" s="336"/>
+      <c r="R4" s="329"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -13278,11 +13281,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="74"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="334">
+      <c r="M40" s="337">
         <f>SUM(M5:M39)</f>
         <v>2772689</v>
       </c>
-      <c r="N40" s="336">
+      <c r="N40" s="339">
         <f>SUM(N5:N39)</f>
         <v>107354</v>
       </c>
@@ -13313,8 +13316,8 @@
       <c r="L41" s="73">
         <v>638.99</v>
       </c>
-      <c r="M41" s="335"/>
-      <c r="N41" s="337"/>
+      <c r="M41" s="338"/>
+      <c r="N41" s="340"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -13560,29 +13563,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="338" t="s">
+      <c r="H53" s="341" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="339"/>
+      <c r="I53" s="342"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="340">
+      <c r="K53" s="343">
         <f>I51+L51</f>
         <v>60691.69</v>
       </c>
-      <c r="L53" s="341"/>
-      <c r="M53" s="342">
+      <c r="L53" s="344"/>
+      <c r="M53" s="345">
         <f>N40+M40</f>
         <v>2880043</v>
       </c>
-      <c r="N53" s="343"/>
+      <c r="N53" s="346"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="344" t="s">
+      <c r="D54" s="347" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="344"/>
+      <c r="E54" s="347"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2844548.31</v>
@@ -13593,22 +13596,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="345" t="s">
+      <c r="D55" s="348" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="345"/>
+      <c r="E55" s="348"/>
       <c r="F55" s="111">
         <v>-2875380.48</v>
       </c>
-      <c r="I55" s="346" t="s">
+      <c r="I55" s="349" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="347"/>
-      <c r="K55" s="348">
+      <c r="J55" s="350"/>
+      <c r="K55" s="351">
         <f>F57+F58+F59</f>
         <v>247554.74000000008</v>
       </c>
-      <c r="L55" s="349"/>
+      <c r="L55" s="352"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -13639,11 +13642,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="350">
+      <c r="K57" s="353">
         <f>-C4</f>
         <v>-149938.81</v>
       </c>
-      <c r="L57" s="351"/>
+      <c r="L57" s="354"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -13660,22 +13663,22 @@
       <c r="C59" s="128">
         <v>44745</v>
       </c>
-      <c r="D59" s="327" t="s">
+      <c r="D59" s="330" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="328"/>
+      <c r="E59" s="331"/>
       <c r="F59" s="129">
         <v>232165.91</v>
       </c>
-      <c r="I59" s="329" t="s">
+      <c r="I59" s="332" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="330"/>
-      <c r="K59" s="331">
+      <c r="J59" s="333"/>
+      <c r="K59" s="334">
         <f>K55+K57</f>
         <v>97615.93000000008</v>
       </c>
-      <c r="L59" s="331"/>
+      <c r="L59" s="334"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -15305,23 +15308,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="314"/>
-      <c r="C1" s="316" t="s">
+      <c r="B1" s="317"/>
+      <c r="C1" s="319" t="s">
         <v>380</v>
       </c>
-      <c r="D1" s="317"/>
-      <c r="E1" s="317"/>
-      <c r="F1" s="317"/>
-      <c r="G1" s="317"/>
-      <c r="H1" s="317"/>
-      <c r="I1" s="317"/>
-      <c r="J1" s="317"/>
-      <c r="K1" s="317"/>
-      <c r="L1" s="317"/>
-      <c r="M1" s="317"/>
+      <c r="D1" s="320"/>
+      <c r="E1" s="320"/>
+      <c r="F1" s="320"/>
+      <c r="G1" s="320"/>
+      <c r="H1" s="320"/>
+      <c r="I1" s="320"/>
+      <c r="J1" s="320"/>
+      <c r="K1" s="320"/>
+      <c r="L1" s="320"/>
+      <c r="M1" s="320"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="315"/>
+      <c r="B2" s="318"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -15331,21 +15334,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="318" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="319"/>
+      <c r="B3" s="321" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="322"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="320" t="s">
+      <c r="H3" s="323" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="320"/>
+      <c r="I3" s="323"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="325" t="s">
+      <c r="R3" s="328" t="s">
         <v>38</v>
       </c>
     </row>
@@ -15360,14 +15363,14 @@
       <c r="D4" s="16">
         <v>44745</v>
       </c>
-      <c r="E4" s="321" t="s">
+      <c r="E4" s="324" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="322"/>
-      <c r="H4" s="323" t="s">
+      <c r="F4" s="325"/>
+      <c r="H4" s="326" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="324"/>
+      <c r="I4" s="327"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -15377,11 +15380,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="332" t="s">
+      <c r="P4" s="335" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="333"/>
-      <c r="R4" s="326"/>
+      <c r="Q4" s="336"/>
+      <c r="R4" s="329"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -16826,11 +16829,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="74"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="334">
+      <c r="M40" s="337">
         <f>SUM(M5:M39)</f>
         <v>2373103</v>
       </c>
-      <c r="N40" s="336">
+      <c r="N40" s="339">
         <f>SUM(N5:N39)</f>
         <v>67308</v>
       </c>
@@ -16859,8 +16862,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="235"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="335"/>
-      <c r="N41" s="337"/>
+      <c r="M41" s="338"/>
+      <c r="N41" s="340"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -17075,29 +17078,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="338" t="s">
+      <c r="H53" s="341" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="339"/>
+      <c r="I53" s="342"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="340">
+      <c r="K53" s="343">
         <f>I51+L51</f>
         <v>79649.720000000016</v>
       </c>
-      <c r="L53" s="341"/>
-      <c r="M53" s="342">
+      <c r="L53" s="344"/>
+      <c r="M53" s="345">
         <f>N40+M40</f>
         <v>2440411</v>
       </c>
-      <c r="N53" s="343"/>
+      <c r="N53" s="346"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="344" t="s">
+      <c r="D54" s="347" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="344"/>
+      <c r="E54" s="347"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2356249.2799999998</v>
@@ -17108,22 +17111,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="345" t="s">
+      <c r="D55" s="348" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="345"/>
+      <c r="E55" s="348"/>
       <c r="F55" s="111">
         <v>-2471332.31</v>
       </c>
-      <c r="I55" s="346" t="s">
+      <c r="I55" s="349" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="347"/>
-      <c r="K55" s="348">
+      <c r="J55" s="350"/>
+      <c r="K55" s="351">
         <f>F57+F58+F59</f>
         <v>214026.38999999972</v>
       </c>
-      <c r="L55" s="349"/>
+      <c r="L55" s="352"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -17154,11 +17157,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="350">
+      <c r="K57" s="353">
         <f>-C4</f>
         <v>-232165.91</v>
       </c>
-      <c r="L57" s="351"/>
+      <c r="L57" s="354"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -17175,22 +17178,22 @@
       <c r="C59" s="128">
         <v>44773</v>
       </c>
-      <c r="D59" s="327" t="s">
+      <c r="D59" s="330" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="328"/>
+      <c r="E59" s="331"/>
       <c r="F59" s="129">
         <v>273736.42</v>
       </c>
-      <c r="I59" s="329" t="s">
+      <c r="I59" s="332" t="s">
         <v>325</v>
       </c>
-      <c r="J59" s="330"/>
-      <c r="K59" s="331">
+      <c r="J59" s="333"/>
+      <c r="K59" s="334">
         <f>K55+K57</f>
         <v>-18139.520000000281</v>
       </c>
-      <c r="L59" s="331"/>
+      <c r="L59" s="334"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -18727,23 +18730,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="314"/>
-      <c r="C1" s="316" t="s">
+      <c r="B1" s="317"/>
+      <c r="C1" s="319" t="s">
         <v>421</v>
       </c>
-      <c r="D1" s="317"/>
-      <c r="E1" s="317"/>
-      <c r="F1" s="317"/>
-      <c r="G1" s="317"/>
-      <c r="H1" s="317"/>
-      <c r="I1" s="317"/>
-      <c r="J1" s="317"/>
-      <c r="K1" s="317"/>
-      <c r="L1" s="317"/>
-      <c r="M1" s="317"/>
+      <c r="D1" s="320"/>
+      <c r="E1" s="320"/>
+      <c r="F1" s="320"/>
+      <c r="G1" s="320"/>
+      <c r="H1" s="320"/>
+      <c r="I1" s="320"/>
+      <c r="J1" s="320"/>
+      <c r="K1" s="320"/>
+      <c r="L1" s="320"/>
+      <c r="M1" s="320"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="315"/>
+      <c r="B2" s="318"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -18753,21 +18756,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="318" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="319"/>
+      <c r="B3" s="321" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="322"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="320" t="s">
+      <c r="H3" s="323" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="320"/>
+      <c r="I3" s="323"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="325" t="s">
+      <c r="R3" s="328" t="s">
         <v>38</v>
       </c>
     </row>
@@ -18782,14 +18785,14 @@
       <c r="D4" s="16">
         <v>44773</v>
       </c>
-      <c r="E4" s="321" t="s">
+      <c r="E4" s="324" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="322"/>
-      <c r="H4" s="323" t="s">
+      <c r="F4" s="325"/>
+      <c r="H4" s="326" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="324"/>
+      <c r="I4" s="327"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -18799,11 +18802,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="332" t="s">
+      <c r="P4" s="335" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="333"/>
-      <c r="R4" s="326"/>
+      <c r="Q4" s="336"/>
+      <c r="R4" s="329"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -20283,11 +20286,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="74"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="334">
+      <c r="M40" s="337">
         <f>SUM(M5:M39)</f>
         <v>2375259</v>
       </c>
-      <c r="N40" s="336">
+      <c r="N40" s="339">
         <f>SUM(N5:N39)</f>
         <v>61117</v>
       </c>
@@ -20316,8 +20319,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="235"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="335"/>
-      <c r="N41" s="337"/>
+      <c r="M41" s="338"/>
+      <c r="N41" s="340"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -20532,29 +20535,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="338" t="s">
+      <c r="H53" s="341" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="339"/>
+      <c r="I53" s="342"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="340">
+      <c r="K53" s="343">
         <f>I51+L51</f>
         <v>52857.25</v>
       </c>
-      <c r="L53" s="341"/>
-      <c r="M53" s="342">
+      <c r="L53" s="344"/>
+      <c r="M53" s="345">
         <f>N40+M40</f>
         <v>2436376</v>
       </c>
-      <c r="N53" s="343"/>
+      <c r="N53" s="346"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="344" t="s">
+      <c r="D54" s="347" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="344"/>
+      <c r="E54" s="347"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2370653.75</v>
@@ -20565,22 +20568,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="345" t="s">
+      <c r="D55" s="348" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="345"/>
+      <c r="E55" s="348"/>
       <c r="F55" s="111">
         <v>-2401197.5699999998</v>
       </c>
-      <c r="I55" s="346" t="s">
+      <c r="I55" s="349" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="347"/>
-      <c r="K55" s="348">
+      <c r="J55" s="350"/>
+      <c r="K55" s="351">
         <f>F57+F58+F59</f>
         <v>259241.77000000016</v>
       </c>
-      <c r="L55" s="349"/>
+      <c r="L55" s="352"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -20611,11 +20614,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="350">
+      <c r="K57" s="353">
         <f>-C4</f>
         <v>-273736.42</v>
       </c>
-      <c r="L57" s="351"/>
+      <c r="L57" s="354"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -20632,22 +20635,22 @@
       <c r="C59" s="128">
         <v>44801</v>
       </c>
-      <c r="D59" s="327" t="s">
+      <c r="D59" s="330" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="328"/>
+      <c r="E59" s="331"/>
       <c r="F59" s="129">
         <v>236400.59</v>
       </c>
-      <c r="I59" s="353" t="s">
+      <c r="I59" s="356" t="s">
         <v>325</v>
       </c>
-      <c r="J59" s="354"/>
-      <c r="K59" s="355">
+      <c r="J59" s="357"/>
+      <c r="K59" s="358">
         <f>K55+K57</f>
         <v>-14494.64999999982</v>
       </c>
-      <c r="L59" s="355"/>
+      <c r="L59" s="358"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -22171,10 +22174,10 @@
   <dimension ref="A1:U81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N29" sqref="N29"/>
+      <selection pane="bottomRight" activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22199,23 +22202,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="314"/>
-      <c r="C1" s="316" t="s">
+      <c r="B1" s="317"/>
+      <c r="C1" s="319" t="s">
         <v>465</v>
       </c>
-      <c r="D1" s="317"/>
-      <c r="E1" s="317"/>
-      <c r="F1" s="317"/>
-      <c r="G1" s="317"/>
-      <c r="H1" s="317"/>
-      <c r="I1" s="317"/>
-      <c r="J1" s="317"/>
-      <c r="K1" s="317"/>
-      <c r="L1" s="317"/>
-      <c r="M1" s="317"/>
+      <c r="D1" s="320"/>
+      <c r="E1" s="320"/>
+      <c r="F1" s="320"/>
+      <c r="G1" s="320"/>
+      <c r="H1" s="320"/>
+      <c r="I1" s="320"/>
+      <c r="J1" s="320"/>
+      <c r="K1" s="320"/>
+      <c r="L1" s="320"/>
+      <c r="M1" s="320"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="315"/>
+      <c r="B2" s="318"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -22225,21 +22228,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="318" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="319"/>
+      <c r="B3" s="321" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="322"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="320" t="s">
+      <c r="H3" s="323" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="320"/>
+      <c r="I3" s="323"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="325" t="s">
+      <c r="R3" s="328" t="s">
         <v>38</v>
       </c>
     </row>
@@ -22254,14 +22257,14 @@
       <c r="D4" s="16">
         <v>44801</v>
       </c>
-      <c r="E4" s="321" t="s">
+      <c r="E4" s="324" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="322"/>
-      <c r="H4" s="323" t="s">
+      <c r="F4" s="325"/>
+      <c r="H4" s="326" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="324"/>
+      <c r="I4" s="327"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -22271,11 +22274,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="332" t="s">
+      <c r="P4" s="335" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="333"/>
-      <c r="R4" s="326"/>
+      <c r="Q4" s="336"/>
+      <c r="R4" s="329"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -22313,7 +22316,7 @@
       <c r="N5" s="31">
         <v>0</v>
       </c>
-      <c r="O5" s="356"/>
+      <c r="O5" s="314"/>
       <c r="P5" s="32">
         <f>N5+M5+L5+I5+C5</f>
         <v>50477.5</v>
@@ -22324,7 +22327,7 @@
       <c r="R5" s="283">
         <v>2558</v>
       </c>
-      <c r="S5" s="357">
+      <c r="S5" s="315">
         <v>44802</v>
       </c>
     </row>
@@ -22359,7 +22362,7 @@
       <c r="N6" s="31">
         <v>3567</v>
       </c>
-      <c r="O6" s="356"/>
+      <c r="O6" s="314"/>
       <c r="P6" s="32">
         <f t="shared" ref="P6:P40" si="0">N6+M6+L6+I6+C6</f>
         <v>91653</v>
@@ -22370,7 +22373,7 @@
       <c r="R6" s="283">
         <v>30160</v>
       </c>
-      <c r="S6" s="357">
+      <c r="S6" s="315">
         <v>44803</v>
       </c>
     </row>
@@ -22408,19 +22411,19 @@
       <c r="N7" s="31">
         <v>50</v>
       </c>
-      <c r="O7" s="356"/>
+      <c r="O7" s="314"/>
       <c r="P7" s="32">
         <f>N7+M7+L7+I7+C7</f>
         <v>36876</v>
       </c>
       <c r="Q7" s="12">
-        <f t="shared" ref="Q6:Q39" si="1">P7-F7</f>
+        <f t="shared" ref="Q7:Q39" si="1">P7-F7</f>
         <v>0</v>
       </c>
       <c r="R7" s="12">
         <v>0</v>
       </c>
-      <c r="S7" s="356">
+      <c r="S7" s="314">
         <v>44804</v>
       </c>
     </row>
@@ -22458,7 +22461,7 @@
       <c r="N8" s="31">
         <v>3482</v>
       </c>
-      <c r="O8" s="356"/>
+      <c r="O8" s="314"/>
       <c r="P8" s="32">
         <f t="shared" si="0"/>
         <v>61899</v>
@@ -22470,7 +22473,7 @@
       <c r="R8" s="12">
         <v>0</v>
       </c>
-      <c r="S8" s="356">
+      <c r="S8" s="314">
         <v>44805</v>
       </c>
     </row>
@@ -22506,7 +22509,7 @@
       <c r="N9" s="31">
         <v>4339</v>
       </c>
-      <c r="O9" s="356"/>
+      <c r="O9" s="314"/>
       <c r="P9" s="32">
         <f t="shared" si="0"/>
         <v>111381</v>
@@ -22518,7 +22521,7 @@
       <c r="R9" s="12">
         <v>0</v>
       </c>
-      <c r="S9" s="356">
+      <c r="S9" s="314">
         <v>44806</v>
       </c>
     </row>
@@ -22560,7 +22563,7 @@
       <c r="N10" s="31">
         <v>7615</v>
       </c>
-      <c r="O10" s="356"/>
+      <c r="O10" s="314"/>
       <c r="P10" s="32">
         <f>N10+M10+L10+I10+C10</f>
         <v>97894</v>
@@ -22571,7 +22574,7 @@
       <c r="R10" s="283">
         <v>4347</v>
       </c>
-      <c r="S10" s="357">
+      <c r="S10" s="315">
         <v>44807</v>
       </c>
       <c r="U10" t="s">
@@ -22611,7 +22614,7 @@
       <c r="N11" s="31">
         <v>826</v>
       </c>
-      <c r="O11" s="356"/>
+      <c r="O11" s="314"/>
       <c r="P11" s="32">
         <f>N11+M11+L11+I11+C11</f>
         <v>139225</v>
@@ -22622,7 +22625,7 @@
       <c r="R11" s="283">
         <v>16320</v>
       </c>
-      <c r="S11" s="356">
+      <c r="S11" s="314">
         <v>44808</v>
       </c>
     </row>
@@ -22659,7 +22662,7 @@
       <c r="N12" s="31">
         <v>1704</v>
       </c>
-      <c r="O12" s="356"/>
+      <c r="O12" s="314"/>
       <c r="P12" s="32">
         <f t="shared" si="0"/>
         <v>70174</v>
@@ -22671,7 +22674,7 @@
       <c r="R12" s="12">
         <v>0</v>
       </c>
-      <c r="S12" s="356">
+      <c r="S12" s="314">
         <v>44809</v>
       </c>
     </row>
@@ -22706,7 +22709,7 @@
       <c r="N13" s="31">
         <v>302</v>
       </c>
-      <c r="O13" s="356"/>
+      <c r="O13" s="314"/>
       <c r="P13" s="32">
         <f t="shared" si="0"/>
         <v>82851</v>
@@ -22718,7 +22721,7 @@
       <c r="R13" s="12">
         <v>0</v>
       </c>
-      <c r="S13" s="356">
+      <c r="S13" s="314">
         <v>44810</v>
       </c>
     </row>
@@ -22752,7 +22755,7 @@
       <c r="N14" s="31">
         <v>0</v>
       </c>
-      <c r="O14" s="356"/>
+      <c r="O14" s="314"/>
       <c r="P14" s="32">
         <f t="shared" si="0"/>
         <v>42033</v>
@@ -22764,7 +22767,7 @@
       <c r="R14" s="12">
         <v>0</v>
       </c>
-      <c r="S14" s="356">
+      <c r="S14" s="314">
         <v>44811</v>
       </c>
     </row>
@@ -22799,7 +22802,7 @@
       <c r="N15" s="31">
         <v>3035</v>
       </c>
-      <c r="O15" s="356"/>
+      <c r="O15" s="314"/>
       <c r="P15" s="32">
         <f t="shared" si="0"/>
         <v>79497</v>
@@ -22811,7 +22814,7 @@
       <c r="R15" s="12">
         <v>0</v>
       </c>
-      <c r="S15" s="356">
+      <c r="S15" s="314">
         <v>44812</v>
       </c>
     </row>
@@ -22848,7 +22851,7 @@
       <c r="N16" s="31">
         <v>722</v>
       </c>
-      <c r="O16" s="356"/>
+      <c r="O16" s="314"/>
       <c r="P16" s="32">
         <f t="shared" si="0"/>
         <v>139439</v>
@@ -22860,7 +22863,7 @@
       <c r="R16" s="12">
         <v>0</v>
       </c>
-      <c r="S16" s="356">
+      <c r="S16" s="314">
         <v>44813</v>
       </c>
     </row>
@@ -22901,7 +22904,7 @@
       <c r="N17" s="31">
         <v>5318</v>
       </c>
-      <c r="O17" s="356"/>
+      <c r="O17" s="314"/>
       <c r="P17" s="32">
         <f t="shared" si="0"/>
         <v>90718</v>
@@ -22913,7 +22916,7 @@
       <c r="R17" s="8">
         <v>0</v>
       </c>
-      <c r="S17" s="356">
+      <c r="S17" s="314">
         <v>44814</v>
       </c>
     </row>
@@ -22948,7 +22951,7 @@
       <c r="N18" s="31">
         <v>500</v>
       </c>
-      <c r="O18" s="356"/>
+      <c r="O18" s="314"/>
       <c r="P18" s="32">
         <f t="shared" si="0"/>
         <v>129054</v>
@@ -22960,7 +22963,7 @@
       <c r="R18" s="8">
         <v>0</v>
       </c>
-      <c r="S18" s="356">
+      <c r="S18" s="314">
         <v>44815</v>
       </c>
     </row>
@@ -22997,7 +23000,7 @@
       <c r="N19" s="31">
         <v>230</v>
       </c>
-      <c r="O19" s="356"/>
+      <c r="O19" s="314"/>
       <c r="P19" s="32">
         <f t="shared" si="0"/>
         <v>77315</v>
@@ -23009,7 +23012,7 @@
       <c r="R19" s="8">
         <v>0</v>
       </c>
-      <c r="S19" s="356">
+      <c r="S19" s="314">
         <v>44816</v>
       </c>
     </row>
@@ -23044,7 +23047,7 @@
       <c r="N20" s="31">
         <v>653</v>
       </c>
-      <c r="O20" s="356"/>
+      <c r="O20" s="314"/>
       <c r="P20" s="32">
         <f t="shared" si="0"/>
         <v>77935</v>
@@ -23056,7 +23059,7 @@
       <c r="R20" s="8">
         <v>0</v>
       </c>
-      <c r="S20" s="356">
+      <c r="S20" s="314">
         <v>44817</v>
       </c>
     </row>
@@ -23091,7 +23094,7 @@
       <c r="N21" s="31">
         <v>12446</v>
       </c>
-      <c r="O21" s="356"/>
+      <c r="O21" s="314"/>
       <c r="P21" s="32">
         <f t="shared" si="0"/>
         <v>112539</v>
@@ -23103,7 +23106,7 @@
       <c r="R21" s="8">
         <v>0</v>
       </c>
-      <c r="S21" s="356">
+      <c r="S21" s="314">
         <v>44818</v>
       </c>
     </row>
@@ -23140,7 +23143,7 @@
       <c r="N22" s="31">
         <v>1357</v>
       </c>
-      <c r="O22" s="356"/>
+      <c r="O22" s="314"/>
       <c r="P22" s="32">
         <f t="shared" si="0"/>
         <v>128781</v>
@@ -23152,7 +23155,7 @@
       <c r="R22" s="8">
         <v>0</v>
       </c>
-      <c r="S22" s="356">
+      <c r="S22" s="314">
         <v>44819</v>
       </c>
     </row>
@@ -23189,7 +23192,7 @@
       <c r="N23" s="31">
         <v>694</v>
       </c>
-      <c r="O23" s="356"/>
+      <c r="O23" s="314"/>
       <c r="P23" s="32">
         <f t="shared" si="0"/>
         <v>93698</v>
@@ -23201,7 +23204,7 @@
       <c r="R23" s="8">
         <v>0</v>
       </c>
-      <c r="S23" s="356">
+      <c r="S23" s="314">
         <v>44820</v>
       </c>
     </row>
@@ -23240,7 +23243,7 @@
       <c r="N24" s="31">
         <v>5429</v>
       </c>
-      <c r="O24" s="356"/>
+      <c r="O24" s="314"/>
       <c r="P24" s="32">
         <f t="shared" si="0"/>
         <v>111198</v>
@@ -23252,7 +23255,7 @@
       <c r="R24" s="8">
         <v>0</v>
       </c>
-      <c r="S24" s="356">
+      <c r="S24" s="314">
         <v>44821</v>
       </c>
     </row>
@@ -23287,7 +23290,7 @@
       <c r="N25" s="31">
         <v>290</v>
       </c>
-      <c r="O25" s="356"/>
+      <c r="O25" s="314"/>
       <c r="P25" s="32">
         <f t="shared" si="0"/>
         <v>145703</v>
@@ -23299,7 +23302,7 @@
       <c r="R25" s="8">
         <v>0</v>
       </c>
-      <c r="S25" s="356">
+      <c r="S25" s="314">
         <v>44822</v>
       </c>
     </row>
@@ -23336,7 +23339,7 @@
       <c r="N26" s="31">
         <v>402</v>
       </c>
-      <c r="O26" s="356"/>
+      <c r="O26" s="314"/>
       <c r="P26" s="32">
         <f t="shared" si="0"/>
         <v>89271</v>
@@ -23348,7 +23351,7 @@
       <c r="R26" s="8">
         <v>0</v>
       </c>
-      <c r="S26" s="356">
+      <c r="S26" s="314">
         <v>44823</v>
       </c>
     </row>
@@ -23383,7 +23386,7 @@
       <c r="N27" s="31">
         <v>0</v>
       </c>
-      <c r="O27" s="356"/>
+      <c r="O27" s="314"/>
       <c r="P27" s="32">
         <f t="shared" si="0"/>
         <v>96379</v>
@@ -23395,7 +23398,7 @@
       <c r="R27" s="8">
         <v>0</v>
       </c>
-      <c r="S27" s="356">
+      <c r="S27" s="314">
         <v>44824</v>
       </c>
     </row>
@@ -23430,7 +23433,7 @@
       <c r="N28" s="31">
         <v>0</v>
       </c>
-      <c r="O28" s="356"/>
+      <c r="O28" s="314"/>
       <c r="P28" s="32">
         <f t="shared" si="0"/>
         <v>71070</v>
@@ -23442,7 +23445,7 @@
       <c r="R28" s="8">
         <v>0</v>
       </c>
-      <c r="S28" s="356">
+      <c r="S28" s="314">
         <v>44825</v>
       </c>
     </row>
@@ -23458,24 +23461,29 @@
       <c r="E29" s="26">
         <v>44826</v>
       </c>
-      <c r="F29" s="27"/>
+      <c r="F29" s="27">
+        <v>98470</v>
+      </c>
       <c r="H29" s="28">
         <v>44826</v>
       </c>
-      <c r="I29" s="29"/>
+      <c r="I29" s="29">
+        <v>1367</v>
+      </c>
       <c r="J29" s="65"/>
       <c r="K29" s="70"/>
       <c r="L29" s="64"/>
       <c r="M29" s="30">
-        <v>0</v>
+        <f>67103+30000</f>
+        <v>97103</v>
       </c>
       <c r="N29" s="31">
         <v>0</v>
       </c>
-      <c r="O29" s="356"/>
+      <c r="O29" s="314"/>
       <c r="P29" s="32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>98470</v>
       </c>
       <c r="Q29" s="12">
         <f t="shared" si="1"/>
@@ -23484,7 +23492,7 @@
       <c r="R29" s="8">
         <v>0</v>
       </c>
-      <c r="S29" s="356">
+      <c r="S29" s="314">
         <v>44826</v>
       </c>
     </row>
@@ -23494,30 +23502,37 @@
         <v>44827</v>
       </c>
       <c r="C30" s="24">
-        <v>0</v>
-      </c>
-      <c r="D30" s="69"/>
+        <v>7793</v>
+      </c>
+      <c r="D30" s="69" t="s">
+        <v>49</v>
+      </c>
       <c r="E30" s="26">
         <v>44827</v>
       </c>
-      <c r="F30" s="27"/>
+      <c r="F30" s="27">
+        <v>117536</v>
+      </c>
       <c r="H30" s="28">
         <v>44827</v>
       </c>
-      <c r="I30" s="29"/>
+      <c r="I30" s="29">
+        <v>100</v>
+      </c>
       <c r="J30" s="71"/>
       <c r="K30" s="72"/>
       <c r="L30" s="73"/>
       <c r="M30" s="30">
-        <v>0</v>
+        <f>55000+34429+20000</f>
+        <v>109429</v>
       </c>
       <c r="N30" s="31">
-        <v>0</v>
-      </c>
-      <c r="O30" s="356"/>
+        <v>214</v>
+      </c>
+      <c r="O30" s="314"/>
       <c r="P30" s="32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>117536</v>
       </c>
       <c r="Q30" s="12">
         <f t="shared" si="1"/>
@@ -23526,7 +23541,7 @@
       <c r="R30" s="8">
         <v>0</v>
       </c>
-      <c r="S30" s="356">
+      <c r="S30" s="314">
         <v>44827</v>
       </c>
     </row>
@@ -23542,24 +23557,35 @@
       <c r="E31" s="26">
         <v>44828</v>
       </c>
-      <c r="F31" s="27"/>
+      <c r="F31" s="27">
+        <v>106553</v>
+      </c>
       <c r="H31" s="28">
         <v>44828</v>
       </c>
-      <c r="I31" s="29"/>
-      <c r="J31" s="71"/>
-      <c r="K31" s="74"/>
-      <c r="L31" s="75"/>
+      <c r="I31" s="29">
+        <v>86</v>
+      </c>
+      <c r="J31" s="71">
+        <v>44828</v>
+      </c>
+      <c r="K31" s="74" t="s">
+        <v>470</v>
+      </c>
+      <c r="L31" s="75">
+        <v>10953</v>
+      </c>
       <c r="M31" s="30">
-        <v>0</v>
+        <f>52305+35000</f>
+        <v>87305</v>
       </c>
       <c r="N31" s="31">
-        <v>0</v>
-      </c>
-      <c r="O31" s="356"/>
+        <v>8209</v>
+      </c>
+      <c r="O31" s="314"/>
       <c r="P31" s="32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>106553</v>
       </c>
       <c r="Q31" s="12">
         <f t="shared" si="1"/>
@@ -23568,7 +23594,7 @@
       <c r="R31" s="8">
         <v>0</v>
       </c>
-      <c r="S31" s="356">
+      <c r="S31" s="314">
         <v>44828</v>
       </c>
     </row>
@@ -23584,24 +23610,29 @@
       <c r="E32" s="26">
         <v>44829</v>
       </c>
-      <c r="F32" s="27"/>
+      <c r="F32" s="27">
+        <v>144028</v>
+      </c>
       <c r="H32" s="28">
         <v>44829</v>
       </c>
-      <c r="I32" s="29"/>
+      <c r="I32" s="29">
+        <v>90</v>
+      </c>
       <c r="J32" s="71"/>
       <c r="K32" s="72"/>
       <c r="L32" s="73"/>
       <c r="M32" s="30">
-        <v>0</v>
+        <f>90000+40000+13302</f>
+        <v>143302</v>
       </c>
       <c r="N32" s="31">
-        <v>0</v>
-      </c>
-      <c r="O32" s="356"/>
+        <v>636</v>
+      </c>
+      <c r="O32" s="314"/>
       <c r="P32" s="32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>144028</v>
       </c>
       <c r="Q32" s="12">
         <f t="shared" si="1"/>
@@ -23610,7 +23641,7 @@
       <c r="R32" s="8">
         <v>0</v>
       </c>
-      <c r="S32" s="356">
+      <c r="S32" s="314">
         <v>44829</v>
       </c>
     </row>
@@ -23620,30 +23651,37 @@
         <v>44830</v>
       </c>
       <c r="C33" s="24">
-        <v>0</v>
-      </c>
-      <c r="D33" s="77"/>
+        <v>5250</v>
+      </c>
+      <c r="D33" s="77" t="s">
+        <v>469</v>
+      </c>
       <c r="E33" s="26">
         <v>44830</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="27">
+        <v>69263</v>
+      </c>
       <c r="H33" s="28">
         <v>44830</v>
       </c>
-      <c r="I33" s="29"/>
+      <c r="I33" s="29">
+        <v>163</v>
+      </c>
       <c r="J33" s="71"/>
       <c r="K33" s="74"/>
       <c r="L33" s="78"/>
       <c r="M33" s="30">
-        <v>0</v>
+        <f>15000+48549</f>
+        <v>63549</v>
       </c>
       <c r="N33" s="31">
-        <v>0</v>
-      </c>
-      <c r="O33" s="356"/>
+        <v>301</v>
+      </c>
+      <c r="O33" s="314"/>
       <c r="P33" s="32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>69263</v>
       </c>
       <c r="Q33" s="12">
         <f t="shared" si="1"/>
@@ -23652,7 +23690,7 @@
       <c r="R33" s="8">
         <v>0</v>
       </c>
-      <c r="S33" s="356">
+      <c r="S33" s="314">
         <v>44830</v>
       </c>
     </row>
@@ -23668,11 +23706,15 @@
       <c r="E34" s="26">
         <v>44831</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="27">
+        <v>78606</v>
+      </c>
       <c r="H34" s="28">
         <v>44831</v>
       </c>
-      <c r="I34" s="29"/>
+      <c r="I34" s="29">
+        <v>35</v>
+      </c>
       <c r="J34" s="71"/>
       <c r="K34" s="79"/>
       <c r="L34" s="80"/>
@@ -23682,18 +23724,18 @@
       <c r="N34" s="31">
         <v>0</v>
       </c>
-      <c r="O34" s="356"/>
+      <c r="O34" s="314"/>
       <c r="P34" s="32">
         <v>0</v>
       </c>
       <c r="Q34" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-78606</v>
       </c>
       <c r="R34" s="8">
         <v>0</v>
       </c>
-      <c r="S34" s="356">
+      <c r="S34" s="314">
         <v>44831</v>
       </c>
     </row>
@@ -23723,7 +23765,7 @@
       <c r="N35" s="31">
         <v>0</v>
       </c>
-      <c r="O35" s="356"/>
+      <c r="O35" s="314"/>
       <c r="P35" s="32">
         <v>0</v>
       </c>
@@ -23731,8 +23773,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R35" s="8"/>
-      <c r="S35" s="356">
+      <c r="R35" s="8">
+        <v>0</v>
+      </c>
+      <c r="S35" s="314">
         <v>44832</v>
       </c>
     </row>
@@ -23762,7 +23806,7 @@
       <c r="N36" s="31">
         <v>0</v>
       </c>
-      <c r="O36" s="356"/>
+      <c r="O36" s="314"/>
       <c r="P36" s="32">
         <v>0</v>
       </c>
@@ -23770,8 +23814,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R36" s="8"/>
-      <c r="S36" s="356">
+      <c r="R36" s="8">
+        <v>0</v>
+      </c>
+      <c r="S36" s="314">
         <v>44833</v>
       </c>
     </row>
@@ -23801,7 +23847,7 @@
       <c r="N37" s="31">
         <v>0</v>
       </c>
-      <c r="O37" s="356"/>
+      <c r="O37" s="314"/>
       <c r="P37" s="32">
         <v>0</v>
       </c>
@@ -23809,7 +23855,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S37" s="356">
+      <c r="R37" s="8">
+        <v>0</v>
+      </c>
+      <c r="S37" s="314">
         <v>44834</v>
       </c>
     </row>
@@ -23839,7 +23888,7 @@
       <c r="N38" s="31">
         <v>0</v>
       </c>
-      <c r="O38" s="356"/>
+      <c r="O38" s="314"/>
       <c r="P38" s="32">
         <v>0</v>
       </c>
@@ -23847,7 +23896,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S38" s="356">
+      <c r="R38" s="8">
+        <v>0</v>
+      </c>
+      <c r="S38" s="314">
         <v>44835</v>
       </c>
     </row>
@@ -23877,7 +23929,7 @@
       <c r="N39" s="31">
         <v>0</v>
       </c>
-      <c r="O39" s="356"/>
+      <c r="O39" s="314"/>
       <c r="P39" s="32">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -23886,7 +23938,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S39" s="356">
+      <c r="R39" s="8">
+        <v>0</v>
+      </c>
+      <c r="S39" s="314">
         <v>44836</v>
       </c>
     </row>
@@ -23904,23 +23959,23 @@
       <c r="J40" s="71"/>
       <c r="K40" s="74"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="334">
+      <c r="M40" s="337">
         <f>SUM(M5:M39)</f>
-        <v>2043551.5</v>
-      </c>
-      <c r="N40" s="336">
+        <v>2544239.5</v>
+      </c>
+      <c r="N40" s="339">
         <f>SUM(N5:N39)</f>
-        <v>52961</v>
+        <v>62321</v>
       </c>
       <c r="P40" s="32">
         <f t="shared" si="0"/>
-        <v>2096512.5</v>
+        <v>2606560.5</v>
       </c>
       <c r="Q40" s="284">
         <f>SUM(Q5:Q39)</f>
-        <v>0</v>
-      </c>
-      <c r="R40" s="358">
+        <v>-78606</v>
+      </c>
+      <c r="R40" s="316">
         <f>SUM(R5:R39)</f>
         <v>53385</v>
       </c>
@@ -23937,8 +23992,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="235"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="335"/>
-      <c r="N41" s="337"/>
+      <c r="M41" s="338"/>
+      <c r="N41" s="340"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -24111,7 +24166,7 @@
       </c>
       <c r="C51" s="102">
         <f>SUM(C5:C50)</f>
-        <v>91923</v>
+        <v>104966</v>
       </c>
       <c r="D51" s="103"/>
       <c r="E51" s="104" t="s">
@@ -24119,7 +24174,7 @@
       </c>
       <c r="F51" s="105">
         <f>SUM(F5:F50)</f>
-        <v>2173676</v>
+        <v>2788132</v>
       </c>
       <c r="G51" s="103"/>
       <c r="H51" s="106" t="s">
@@ -24127,7 +24182,7 @@
       </c>
       <c r="I51" s="107">
         <f>SUM(I5:I50)</f>
-        <v>2844</v>
+        <v>4685</v>
       </c>
       <c r="J51" s="108"/>
       <c r="K51" s="109" t="s">
@@ -24135,7 +24190,7 @@
       </c>
       <c r="L51" s="110">
         <f>SUM(L5:L50)</f>
-        <v>35781</v>
+        <v>46734</v>
       </c>
       <c r="M51" s="111"/>
       <c r="N51" s="111"/>
@@ -24153,32 +24208,32 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="338" t="s">
+      <c r="H53" s="341" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="339"/>
+      <c r="I53" s="342"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="340">
+      <c r="K53" s="343">
         <f>I51+L51</f>
-        <v>38625</v>
-      </c>
-      <c r="L53" s="341"/>
-      <c r="M53" s="342">
+        <v>51419</v>
+      </c>
+      <c r="L53" s="344"/>
+      <c r="M53" s="345">
         <f>N40+M40</f>
-        <v>2096512.5</v>
-      </c>
-      <c r="N53" s="343"/>
+        <v>2606560.5</v>
+      </c>
+      <c r="N53" s="346"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="344" t="s">
+      <c r="D54" s="347" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="344"/>
+      <c r="E54" s="347"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
-        <v>2043128</v>
+        <v>2631747</v>
       </c>
       <c r="I54" s="116"/>
       <c r="J54" s="117"/>
@@ -24186,22 +24241,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="345" t="s">
+      <c r="D55" s="348" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="345"/>
+      <c r="E55" s="348"/>
       <c r="F55" s="111">
         <v>0</v>
       </c>
-      <c r="I55" s="346" t="s">
+      <c r="I55" s="349" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="347"/>
-      <c r="K55" s="348">
+      <c r="J55" s="350"/>
+      <c r="K55" s="351">
         <f>F57+F58+F59</f>
-        <v>2043128</v>
-      </c>
-      <c r="L55" s="349"/>
+        <v>2631747</v>
+      </c>
+      <c r="L55" s="352"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -24225,18 +24280,18 @@
       </c>
       <c r="F57" s="111">
         <f>SUM(F54:F56)</f>
-        <v>2043128</v>
+        <v>2631747</v>
       </c>
       <c r="H57" s="22"/>
       <c r="I57" s="124" t="s">
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="350">
+      <c r="K57" s="353">
         <f>-C4</f>
         <v>-236400.59</v>
       </c>
-      <c r="L57" s="351"/>
+      <c r="L57" s="354"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -24251,22 +24306,22 @@
     </row>
     <row r="59" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C59" s="128"/>
-      <c r="D59" s="327" t="s">
+      <c r="D59" s="330" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="328"/>
+      <c r="E59" s="331"/>
       <c r="F59" s="129">
         <v>0</v>
       </c>
-      <c r="I59" s="353" t="s">
+      <c r="I59" s="356" t="s">
         <v>325</v>
       </c>
-      <c r="J59" s="354"/>
-      <c r="K59" s="355">
+      <c r="J59" s="357"/>
+      <c r="K59" s="358">
         <f>K55+K57</f>
-        <v>1806727.41</v>
-      </c>
-      <c r="L59" s="355"/>
+        <v>2395346.41</v>
+      </c>
+      <c r="L59" s="358"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -27313,23 +27368,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="314"/>
-      <c r="C1" s="316" t="s">
+      <c r="B1" s="317"/>
+      <c r="C1" s="319" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="317"/>
-      <c r="E1" s="317"/>
-      <c r="F1" s="317"/>
-      <c r="G1" s="317"/>
-      <c r="H1" s="317"/>
-      <c r="I1" s="317"/>
-      <c r="J1" s="317"/>
-      <c r="K1" s="317"/>
-      <c r="L1" s="317"/>
-      <c r="M1" s="317"/>
+      <c r="D1" s="320"/>
+      <c r="E1" s="320"/>
+      <c r="F1" s="320"/>
+      <c r="G1" s="320"/>
+      <c r="H1" s="320"/>
+      <c r="I1" s="320"/>
+      <c r="J1" s="320"/>
+      <c r="K1" s="320"/>
+      <c r="L1" s="320"/>
+      <c r="M1" s="320"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="315"/>
+      <c r="B2" s="318"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -27339,21 +27394,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="318" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="319"/>
+      <c r="B3" s="321" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="322"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="320" t="s">
+      <c r="H3" s="323" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="320"/>
+      <c r="I3" s="323"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="325" t="s">
+      <c r="R3" s="328" t="s">
         <v>38</v>
       </c>
     </row>
@@ -27368,14 +27423,14 @@
       <c r="D4" s="16">
         <v>44591</v>
       </c>
-      <c r="E4" s="321" t="s">
+      <c r="E4" s="324" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="322"/>
-      <c r="H4" s="323" t="s">
+      <c r="F4" s="325"/>
+      <c r="H4" s="326" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="324"/>
+      <c r="I4" s="327"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -27385,11 +27440,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="332" t="s">
+      <c r="P4" s="335" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="333"/>
-      <c r="R4" s="326"/>
+      <c r="Q4" s="336"/>
+      <c r="R4" s="329"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -28826,11 +28881,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="87"/>
       <c r="L40" s="78"/>
-      <c r="M40" s="352">
+      <c r="M40" s="355">
         <f>SUM(M5:M39)</f>
         <v>1636108</v>
       </c>
-      <c r="N40" s="336">
+      <c r="N40" s="339">
         <f>SUM(N5:N39)</f>
         <v>55675</v>
       </c>
@@ -28855,8 +28910,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="74"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="335"/>
-      <c r="N41" s="337"/>
+      <c r="M41" s="338"/>
+      <c r="N41" s="340"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -29063,29 +29118,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="338" t="s">
+      <c r="H53" s="341" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="339"/>
+      <c r="I53" s="342"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="340">
+      <c r="K53" s="343">
         <f>I51+L51</f>
         <v>45634.280000000006</v>
       </c>
-      <c r="L53" s="341"/>
-      <c r="M53" s="342">
+      <c r="L53" s="344"/>
+      <c r="M53" s="345">
         <f>N40+M40</f>
         <v>1691783</v>
       </c>
-      <c r="N53" s="343"/>
+      <c r="N53" s="346"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="344" t="s">
+      <c r="D54" s="347" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="344"/>
+      <c r="E54" s="347"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>1686442.72</v>
@@ -29096,22 +29151,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="345" t="s">
+      <c r="D55" s="348" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="345"/>
+      <c r="E55" s="348"/>
       <c r="F55" s="111">
         <v>-1631962.77</v>
       </c>
-      <c r="I55" s="346" t="s">
+      <c r="I55" s="349" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="347"/>
-      <c r="K55" s="348">
+      <c r="J55" s="350"/>
+      <c r="K55" s="351">
         <f>F57+F58+F59</f>
         <v>238822.13999999996</v>
       </c>
-      <c r="L55" s="349"/>
+      <c r="L55" s="352"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -29142,11 +29197,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="350">
+      <c r="K57" s="353">
         <f>-C4</f>
         <v>-154314.51999999999</v>
       </c>
-      <c r="L57" s="351"/>
+      <c r="L57" s="354"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -29163,22 +29218,22 @@
       <c r="C59" s="128">
         <v>44619</v>
       </c>
-      <c r="D59" s="327" t="s">
+      <c r="D59" s="330" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="328"/>
+      <c r="E59" s="331"/>
       <c r="F59" s="129">
         <v>184342.19</v>
       </c>
-      <c r="I59" s="329" t="s">
+      <c r="I59" s="332" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="330"/>
-      <c r="K59" s="331">
+      <c r="J59" s="333"/>
+      <c r="K59" s="334">
         <f>K55+K57</f>
         <v>84507.619999999966</v>
       </c>
-      <c r="L59" s="331"/>
+      <c r="L59" s="334"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -30628,23 +30683,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="314"/>
-      <c r="C1" s="316" t="s">
+      <c r="B1" s="317"/>
+      <c r="C1" s="319" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="317"/>
-      <c r="E1" s="317"/>
-      <c r="F1" s="317"/>
-      <c r="G1" s="317"/>
-      <c r="H1" s="317"/>
-      <c r="I1" s="317"/>
-      <c r="J1" s="317"/>
-      <c r="K1" s="317"/>
-      <c r="L1" s="317"/>
-      <c r="M1" s="317"/>
+      <c r="D1" s="320"/>
+      <c r="E1" s="320"/>
+      <c r="F1" s="320"/>
+      <c r="G1" s="320"/>
+      <c r="H1" s="320"/>
+      <c r="I1" s="320"/>
+      <c r="J1" s="320"/>
+      <c r="K1" s="320"/>
+      <c r="L1" s="320"/>
+      <c r="M1" s="320"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="315"/>
+      <c r="B2" s="318"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -30654,21 +30709,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="318" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="319"/>
+      <c r="B3" s="321" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="322"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="320" t="s">
+      <c r="H3" s="323" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="320"/>
+      <c r="I3" s="323"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="325" t="s">
+      <c r="R3" s="328" t="s">
         <v>38</v>
       </c>
     </row>
@@ -30683,14 +30738,14 @@
       <c r="D4" s="16">
         <v>44619</v>
       </c>
-      <c r="E4" s="321" t="s">
+      <c r="E4" s="324" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="322"/>
-      <c r="H4" s="323" t="s">
+      <c r="F4" s="325"/>
+      <c r="H4" s="326" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="324"/>
+      <c r="I4" s="327"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -30700,11 +30755,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="332" t="s">
+      <c r="P4" s="335" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="333"/>
-      <c r="R4" s="326"/>
+      <c r="Q4" s="336"/>
+      <c r="R4" s="329"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -32155,11 +32210,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="87"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="334">
+      <c r="M40" s="337">
         <f>SUM(M5:M39)</f>
         <v>1793435</v>
       </c>
-      <c r="N40" s="336">
+      <c r="N40" s="339">
         <f>SUM(N5:N39)</f>
         <v>63995</v>
       </c>
@@ -32184,8 +32239,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="235"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="335"/>
-      <c r="N41" s="337"/>
+      <c r="M41" s="338"/>
+      <c r="N41" s="340"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -32324,29 +32379,29 @@
       <c r="A49" s="33"/>
       <c r="B49" s="113"/>
       <c r="C49" s="1"/>
-      <c r="H49" s="338" t="s">
+      <c r="H49" s="341" t="s">
         <v>12</v>
       </c>
-      <c r="I49" s="339"/>
+      <c r="I49" s="342"/>
       <c r="J49" s="114"/>
-      <c r="K49" s="340">
+      <c r="K49" s="343">
         <f>I47+L47</f>
         <v>90434.03</v>
       </c>
-      <c r="L49" s="341"/>
-      <c r="M49" s="342">
+      <c r="L49" s="344"/>
+      <c r="M49" s="345">
         <f>N40+M40</f>
         <v>1857430</v>
       </c>
-      <c r="N49" s="343"/>
+      <c r="N49" s="346"/>
       <c r="P49" s="32"/>
       <c r="Q49" s="8"/>
     </row>
     <row r="50" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D50" s="344" t="s">
+      <c r="D50" s="347" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="344"/>
+      <c r="E50" s="347"/>
       <c r="F50" s="115">
         <f>F47-K49-C47</f>
         <v>1824260.97</v>
@@ -32357,22 +32412,22 @@
       <c r="Q50" s="8"/>
     </row>
     <row r="51" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D51" s="345" t="s">
+      <c r="D51" s="348" t="s">
         <v>14</v>
       </c>
-      <c r="E51" s="345"/>
+      <c r="E51" s="348"/>
       <c r="F51" s="111">
         <v>-1848136.64</v>
       </c>
-      <c r="I51" s="346" t="s">
+      <c r="I51" s="349" t="s">
         <v>15</v>
       </c>
-      <c r="J51" s="347"/>
-      <c r="K51" s="348">
+      <c r="J51" s="350"/>
+      <c r="K51" s="351">
         <f>F53+F54+F55</f>
         <v>195541.70000000007</v>
       </c>
-      <c r="L51" s="349"/>
+      <c r="L51" s="352"/>
       <c r="P51" s="32"/>
       <c r="Q51" s="8"/>
     </row>
@@ -32403,11 +32458,11 @@
         <v>17</v>
       </c>
       <c r="J53" s="125"/>
-      <c r="K53" s="350">
+      <c r="K53" s="353">
         <f>-C4</f>
         <v>-184342.19</v>
       </c>
-      <c r="L53" s="351"/>
+      <c r="L53" s="354"/>
     </row>
     <row r="54" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D54" s="126" t="s">
@@ -32424,22 +32479,22 @@
       <c r="C55" s="128">
         <v>44647</v>
       </c>
-      <c r="D55" s="327" t="s">
+      <c r="D55" s="330" t="s">
         <v>20</v>
       </c>
-      <c r="E55" s="328"/>
+      <c r="E55" s="331"/>
       <c r="F55" s="129">
         <v>219417.37</v>
       </c>
-      <c r="I55" s="329" t="s">
+      <c r="I55" s="332" t="s">
         <v>226</v>
       </c>
-      <c r="J55" s="330"/>
-      <c r="K55" s="331">
+      <c r="J55" s="333"/>
+      <c r="K55" s="334">
         <f>K51+K53</f>
         <v>11199.510000000068</v>
       </c>
-      <c r="L55" s="331"/>
+      <c r="L55" s="334"/>
     </row>
     <row r="56" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C56" s="130"/>
@@ -34062,23 +34117,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="314"/>
-      <c r="C1" s="316" t="s">
+      <c r="B1" s="317"/>
+      <c r="C1" s="319" t="s">
         <v>225</v>
       </c>
-      <c r="D1" s="317"/>
-      <c r="E1" s="317"/>
-      <c r="F1" s="317"/>
-      <c r="G1" s="317"/>
-      <c r="H1" s="317"/>
-      <c r="I1" s="317"/>
-      <c r="J1" s="317"/>
-      <c r="K1" s="317"/>
-      <c r="L1" s="317"/>
-      <c r="M1" s="317"/>
+      <c r="D1" s="320"/>
+      <c r="E1" s="320"/>
+      <c r="F1" s="320"/>
+      <c r="G1" s="320"/>
+      <c r="H1" s="320"/>
+      <c r="I1" s="320"/>
+      <c r="J1" s="320"/>
+      <c r="K1" s="320"/>
+      <c r="L1" s="320"/>
+      <c r="M1" s="320"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="315"/>
+      <c r="B2" s="318"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -34088,21 +34143,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="318" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="319"/>
+      <c r="B3" s="321" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="322"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="320" t="s">
+      <c r="H3" s="323" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="320"/>
+      <c r="I3" s="323"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="325" t="s">
+      <c r="R3" s="328" t="s">
         <v>38</v>
       </c>
     </row>
@@ -34117,14 +34172,14 @@
       <c r="D4" s="16">
         <v>44647</v>
       </c>
-      <c r="E4" s="321" t="s">
+      <c r="E4" s="324" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="322"/>
-      <c r="H4" s="323" t="s">
+      <c r="F4" s="325"/>
+      <c r="H4" s="326" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="324"/>
+      <c r="I4" s="327"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -34134,11 +34189,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="332" t="s">
+      <c r="P4" s="335" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="333"/>
-      <c r="R4" s="326"/>
+      <c r="Q4" s="336"/>
+      <c r="R4" s="329"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -35735,11 +35790,11 @@
         <f>927.48+128</f>
         <v>1055.48</v>
       </c>
-      <c r="M40" s="334">
+      <c r="M40" s="337">
         <f>SUM(M5:M39)</f>
         <v>2146671</v>
       </c>
-      <c r="N40" s="336">
+      <c r="N40" s="339">
         <f>SUM(N5:N39)</f>
         <v>68590</v>
       </c>
@@ -35770,8 +35825,8 @@
       <c r="L41" s="73">
         <v>1195.68</v>
       </c>
-      <c r="M41" s="335"/>
-      <c r="N41" s="337"/>
+      <c r="M41" s="338"/>
+      <c r="N41" s="340"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -36002,29 +36057,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="338" t="s">
+      <c r="H53" s="341" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="339"/>
+      <c r="I53" s="342"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="340">
+      <c r="K53" s="343">
         <f>I51+L51</f>
         <v>91272.77</v>
       </c>
-      <c r="L53" s="341"/>
-      <c r="M53" s="342">
+      <c r="L53" s="344"/>
+      <c r="M53" s="345">
         <f>N40+M40</f>
         <v>2215261</v>
       </c>
-      <c r="N53" s="343"/>
+      <c r="N53" s="346"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="344" t="s">
+      <c r="D54" s="347" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="344"/>
+      <c r="E54" s="347"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2179879.23</v>
@@ -36035,22 +36090,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="345" t="s">
+      <c r="D55" s="348" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="345"/>
+      <c r="E55" s="348"/>
       <c r="F55" s="111">
         <v>-2227493.48</v>
       </c>
-      <c r="I55" s="346" t="s">
+      <c r="I55" s="349" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="347"/>
-      <c r="K55" s="348">
+      <c r="J55" s="350"/>
+      <c r="K55" s="351">
         <f>F57+F58+F59</f>
         <v>261521.34000000003</v>
       </c>
-      <c r="L55" s="349"/>
+      <c r="L55" s="352"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -36081,11 +36136,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="350">
+      <c r="K57" s="353">
         <f>-C4</f>
         <v>-219417.37</v>
       </c>
-      <c r="L57" s="351"/>
+      <c r="L57" s="354"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -36102,22 +36157,22 @@
       <c r="C59" s="128">
         <v>44682</v>
       </c>
-      <c r="D59" s="327" t="s">
+      <c r="D59" s="330" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="328"/>
+      <c r="E59" s="331"/>
       <c r="F59" s="129">
         <v>297874.59000000003</v>
       </c>
-      <c r="I59" s="329" t="s">
+      <c r="I59" s="332" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="330"/>
-      <c r="K59" s="331">
+      <c r="J59" s="333"/>
+      <c r="K59" s="334">
         <f>K55+K57</f>
         <v>42103.97000000003</v>
       </c>
-      <c r="L59" s="331"/>
+      <c r="L59" s="334"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -37769,23 +37824,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="314"/>
-      <c r="C1" s="316" t="s">
+      <c r="B1" s="317"/>
+      <c r="C1" s="319" t="s">
         <v>277</v>
       </c>
-      <c r="D1" s="317"/>
-      <c r="E1" s="317"/>
-      <c r="F1" s="317"/>
-      <c r="G1" s="317"/>
-      <c r="H1" s="317"/>
-      <c r="I1" s="317"/>
-      <c r="J1" s="317"/>
-      <c r="K1" s="317"/>
-      <c r="L1" s="317"/>
-      <c r="M1" s="317"/>
+      <c r="D1" s="320"/>
+      <c r="E1" s="320"/>
+      <c r="F1" s="320"/>
+      <c r="G1" s="320"/>
+      <c r="H1" s="320"/>
+      <c r="I1" s="320"/>
+      <c r="J1" s="320"/>
+      <c r="K1" s="320"/>
+      <c r="L1" s="320"/>
+      <c r="M1" s="320"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="315"/>
+      <c r="B2" s="318"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -37795,21 +37850,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="318" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="319"/>
+      <c r="B3" s="321" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="322"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="320" t="s">
+      <c r="H3" s="323" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="320"/>
+      <c r="I3" s="323"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="325" t="s">
+      <c r="R3" s="328" t="s">
         <v>38</v>
       </c>
     </row>
@@ -37824,14 +37879,14 @@
       <c r="D4" s="16">
         <v>44682</v>
       </c>
-      <c r="E4" s="321" t="s">
+      <c r="E4" s="324" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="322"/>
-      <c r="H4" s="323" t="s">
+      <c r="F4" s="325"/>
+      <c r="H4" s="326" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="324"/>
+      <c r="I4" s="327"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -37841,11 +37896,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="332" t="s">
+      <c r="P4" s="335" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="333"/>
-      <c r="R4" s="326"/>
+      <c r="Q4" s="336"/>
+      <c r="R4" s="329"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -39362,11 +39417,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="74"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="334">
+      <c r="M40" s="337">
         <f>SUM(M5:M39)</f>
         <v>2144215</v>
       </c>
-      <c r="N40" s="336">
+      <c r="N40" s="339">
         <f>SUM(N5:N39)</f>
         <v>62525</v>
       </c>
@@ -39391,8 +39446,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="235"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="335"/>
-      <c r="N41" s="337"/>
+      <c r="M41" s="338"/>
+      <c r="N41" s="340"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -39603,29 +39658,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="338" t="s">
+      <c r="H53" s="341" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="339"/>
+      <c r="I53" s="342"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="340">
+      <c r="K53" s="343">
         <f>I51+L51</f>
         <v>51231.42</v>
       </c>
-      <c r="L53" s="341"/>
-      <c r="M53" s="342">
+      <c r="L53" s="344"/>
+      <c r="M53" s="345">
         <f>N40+M40</f>
         <v>2206740</v>
       </c>
-      <c r="N53" s="343"/>
+      <c r="N53" s="346"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="344" t="s">
+      <c r="D54" s="347" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="344"/>
+      <c r="E54" s="347"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2189405.58</v>
@@ -39636,22 +39691,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="345" t="s">
+      <c r="D55" s="348" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="345"/>
+      <c r="E55" s="348"/>
       <c r="F55" s="111">
         <v>-2251924.65</v>
       </c>
-      <c r="I55" s="346" t="s">
+      <c r="I55" s="349" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="347"/>
-      <c r="K55" s="348">
+      <c r="J55" s="350"/>
+      <c r="K55" s="351">
         <f>F57+F58+F59</f>
         <v>112552.74000000017</v>
       </c>
-      <c r="L55" s="349"/>
+      <c r="L55" s="352"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -39682,11 +39737,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="350">
+      <c r="K57" s="353">
         <f>-C4</f>
         <v>-297874.59000000003</v>
       </c>
-      <c r="L57" s="351"/>
+      <c r="L57" s="354"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -39703,22 +39758,22 @@
       <c r="C59" s="128">
         <v>44710</v>
       </c>
-      <c r="D59" s="327" t="s">
+      <c r="D59" s="330" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="328"/>
+      <c r="E59" s="331"/>
       <c r="F59" s="129">
         <v>149938.81</v>
       </c>
-      <c r="I59" s="329" t="s">
+      <c r="I59" s="332" t="s">
         <v>325</v>
       </c>
-      <c r="J59" s="330"/>
-      <c r="K59" s="331">
+      <c r="J59" s="333"/>
+      <c r="K59" s="334">
         <f>K55+K57</f>
         <v>-185321.84999999986</v>
       </c>
-      <c r="L59" s="331"/>
+      <c r="L59" s="334"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>

</xml_diff>

<commit_message>
CIERRE  12 OCT 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #09 SEPTIEMBRE 2022/BALANCE   HERRADURA SEPTIEMBRE      2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #09 SEPTIEMBRE 2022/BALANCE   HERRADURA SEPTIEMBRE      2022.xlsx
@@ -572,7 +572,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="512">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -2004,6 +2004,123 @@
   </si>
   <si>
     <t>NOMINA # 40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                    </t>
+  </si>
+  <si>
+    <t>D-08694</t>
+  </si>
+  <si>
+    <t>D-08916</t>
+  </si>
+  <si>
+    <t>D-08970</t>
+  </si>
+  <si>
+    <t>D-08974</t>
+  </si>
+  <si>
+    <t>D-08990</t>
+  </si>
+  <si>
+    <t>D-09060</t>
+  </si>
+  <si>
+    <t>D-09144</t>
+  </si>
+  <si>
+    <t>D-09210</t>
+  </si>
+  <si>
+    <t>D-09326</t>
+  </si>
+  <si>
+    <t>D-09397</t>
+  </si>
+  <si>
+    <t>D-09591</t>
+  </si>
+  <si>
+    <t>D-09594</t>
+  </si>
+  <si>
+    <t>D-09762</t>
+  </si>
+  <si>
+    <t>D-10037</t>
+  </si>
+  <si>
+    <t>D-10038</t>
+  </si>
+  <si>
+    <t>D-10125</t>
+  </si>
+  <si>
+    <t>D-10198</t>
+  </si>
+  <si>
+    <t>D-10378</t>
+  </si>
+  <si>
+    <t>D-10511</t>
+  </si>
+  <si>
+    <t>D-10686</t>
+  </si>
+  <si>
+    <t>D-10761</t>
+  </si>
+  <si>
+    <t>D-10868</t>
+  </si>
+  <si>
+    <t>D-10873</t>
+  </si>
+  <si>
+    <t>D-10946</t>
+  </si>
+  <si>
+    <t>D-10956</t>
+  </si>
+  <si>
+    <t>D-10999</t>
+  </si>
+  <si>
+    <t>D-11062</t>
+  </si>
+  <si>
+    <t>D-11231</t>
+  </si>
+  <si>
+    <t>D-11277</t>
+  </si>
+  <si>
+    <t>D-11509</t>
+  </si>
+  <si>
+    <t>D-11570</t>
+  </si>
+  <si>
+    <t>D-11626</t>
+  </si>
+  <si>
+    <t>D-11797</t>
+  </si>
+  <si>
+    <t>D11938</t>
+  </si>
+  <si>
+    <t>D-12034</t>
+  </si>
+  <si>
+    <t>D-12134</t>
+  </si>
+  <si>
+    <t>D-12242</t>
+  </si>
+  <si>
+    <t>D-12395</t>
   </si>
 </sst>
 </file>
@@ -3350,7 +3467,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="359">
+  <cellXfs count="362">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -3920,6 +4037,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="7" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="19" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4045,6 +4165,12 @@
     </xf>
     <xf numFmtId="166" fontId="12" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8200,23 +8326,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="317"/>
-      <c r="C1" s="319" t="s">
+      <c r="B1" s="318"/>
+      <c r="C1" s="320" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="320"/>
-      <c r="E1" s="320"/>
-      <c r="F1" s="320"/>
-      <c r="G1" s="320"/>
-      <c r="H1" s="320"/>
-      <c r="I1" s="320"/>
-      <c r="J1" s="320"/>
-      <c r="K1" s="320"/>
-      <c r="L1" s="320"/>
-      <c r="M1" s="320"/>
+      <c r="D1" s="321"/>
+      <c r="E1" s="321"/>
+      <c r="F1" s="321"/>
+      <c r="G1" s="321"/>
+      <c r="H1" s="321"/>
+      <c r="I1" s="321"/>
+      <c r="J1" s="321"/>
+      <c r="K1" s="321"/>
+      <c r="L1" s="321"/>
+      <c r="M1" s="321"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="318"/>
+      <c r="B2" s="319"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -8226,21 +8352,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="321" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="322"/>
+      <c r="B3" s="322" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="323"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="323" t="s">
+      <c r="H3" s="324" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="323"/>
+      <c r="I3" s="324"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="328" t="s">
+      <c r="R3" s="329" t="s">
         <v>38</v>
       </c>
     </row>
@@ -8255,14 +8381,14 @@
       <c r="D4" s="16">
         <v>44563</v>
       </c>
-      <c r="E4" s="324" t="s">
+      <c r="E4" s="325" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="325"/>
-      <c r="H4" s="326" t="s">
+      <c r="F4" s="326"/>
+      <c r="H4" s="327" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="327"/>
+      <c r="I4" s="328"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -8272,11 +8398,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="335" t="s">
+      <c r="P4" s="336" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="336"/>
-      <c r="R4" s="329"/>
+      <c r="Q4" s="337"/>
+      <c r="R4" s="330"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -9731,11 +9857,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="87"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="337">
+      <c r="M40" s="338">
         <f>SUM(M5:M39)</f>
         <v>1527030</v>
       </c>
-      <c r="N40" s="339">
+      <c r="N40" s="340">
         <f>SUM(N5:N39)</f>
         <v>50013</v>
       </c>
@@ -9760,8 +9886,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="74"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="338"/>
-      <c r="N41" s="340"/>
+      <c r="M41" s="339"/>
+      <c r="N41" s="341"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -9968,29 +10094,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="341" t="s">
+      <c r="H53" s="342" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="342"/>
+      <c r="I53" s="343"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="343">
+      <c r="K53" s="344">
         <f>I51+L51</f>
         <v>50143.28</v>
       </c>
-      <c r="L53" s="344"/>
-      <c r="M53" s="345">
+      <c r="L53" s="345"/>
+      <c r="M53" s="346">
         <f>N40+M40</f>
         <v>1577043</v>
       </c>
-      <c r="N53" s="346"/>
+      <c r="N53" s="347"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="347" t="s">
+      <c r="D54" s="348" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="347"/>
+      <c r="E54" s="348"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>1561421.72</v>
@@ -10001,22 +10127,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="348" t="s">
+      <c r="D55" s="349" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="348"/>
+      <c r="E55" s="349"/>
       <c r="F55" s="111">
         <v>-1419082.77</v>
       </c>
-      <c r="I55" s="349" t="s">
+      <c r="I55" s="350" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="350"/>
-      <c r="K55" s="351">
+      <c r="J55" s="351"/>
+      <c r="K55" s="352">
         <f>F57+F58+F59</f>
         <v>296963.46999999997</v>
       </c>
-      <c r="L55" s="352"/>
+      <c r="L55" s="353"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -10047,11 +10173,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="353">
+      <c r="K57" s="354">
         <f>-C4</f>
         <v>-221059.7</v>
       </c>
-      <c r="L57" s="354"/>
+      <c r="L57" s="355"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -10068,22 +10194,22 @@
       <c r="C59" s="128">
         <v>44591</v>
       </c>
-      <c r="D59" s="330" t="s">
+      <c r="D59" s="331" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="331"/>
+      <c r="E59" s="332"/>
       <c r="F59" s="129">
         <v>154314.51999999999</v>
       </c>
-      <c r="I59" s="332" t="s">
+      <c r="I59" s="333" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="333"/>
-      <c r="K59" s="334">
+      <c r="J59" s="334"/>
+      <c r="K59" s="335">
         <f>K55+K57</f>
         <v>75903.76999999996</v>
       </c>
-      <c r="L59" s="334"/>
+      <c r="L59" s="335"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -11681,23 +11807,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="317"/>
-      <c r="C1" s="319" t="s">
+      <c r="B1" s="318"/>
+      <c r="C1" s="320" t="s">
         <v>326</v>
       </c>
-      <c r="D1" s="320"/>
-      <c r="E1" s="320"/>
-      <c r="F1" s="320"/>
-      <c r="G1" s="320"/>
-      <c r="H1" s="320"/>
-      <c r="I1" s="320"/>
-      <c r="J1" s="320"/>
-      <c r="K1" s="320"/>
-      <c r="L1" s="320"/>
-      <c r="M1" s="320"/>
+      <c r="D1" s="321"/>
+      <c r="E1" s="321"/>
+      <c r="F1" s="321"/>
+      <c r="G1" s="321"/>
+      <c r="H1" s="321"/>
+      <c r="I1" s="321"/>
+      <c r="J1" s="321"/>
+      <c r="K1" s="321"/>
+      <c r="L1" s="321"/>
+      <c r="M1" s="321"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="318"/>
+      <c r="B2" s="319"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -11707,21 +11833,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="321" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="322"/>
+      <c r="B3" s="322" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="323"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="323" t="s">
+      <c r="H3" s="324" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="323"/>
+      <c r="I3" s="324"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="328" t="s">
+      <c r="R3" s="329" t="s">
         <v>38</v>
       </c>
     </row>
@@ -11736,14 +11862,14 @@
       <c r="D4" s="16">
         <v>44710</v>
       </c>
-      <c r="E4" s="324" t="s">
+      <c r="E4" s="325" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="325"/>
-      <c r="H4" s="326" t="s">
+      <c r="F4" s="326"/>
+      <c r="H4" s="327" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="327"/>
+      <c r="I4" s="328"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -11753,11 +11879,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="335" t="s">
+      <c r="P4" s="336" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="336"/>
-      <c r="R4" s="329"/>
+      <c r="Q4" s="337"/>
+      <c r="R4" s="330"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -13287,11 +13413,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="74"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="337">
+      <c r="M40" s="338">
         <f>SUM(M5:M39)</f>
         <v>2772689</v>
       </c>
-      <c r="N40" s="339">
+      <c r="N40" s="340">
         <f>SUM(N5:N39)</f>
         <v>107354</v>
       </c>
@@ -13322,8 +13448,8 @@
       <c r="L41" s="73">
         <v>638.99</v>
       </c>
-      <c r="M41" s="338"/>
-      <c r="N41" s="340"/>
+      <c r="M41" s="339"/>
+      <c r="N41" s="341"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -13569,29 +13695,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="341" t="s">
+      <c r="H53" s="342" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="342"/>
+      <c r="I53" s="343"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="343">
+      <c r="K53" s="344">
         <f>I51+L51</f>
         <v>60691.69</v>
       </c>
-      <c r="L53" s="344"/>
-      <c r="M53" s="345">
+      <c r="L53" s="345"/>
+      <c r="M53" s="346">
         <f>N40+M40</f>
         <v>2880043</v>
       </c>
-      <c r="N53" s="346"/>
+      <c r="N53" s="347"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="347" t="s">
+      <c r="D54" s="348" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="347"/>
+      <c r="E54" s="348"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2844548.31</v>
@@ -13602,22 +13728,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="348" t="s">
+      <c r="D55" s="349" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="348"/>
+      <c r="E55" s="349"/>
       <c r="F55" s="111">
         <v>-2875380.48</v>
       </c>
-      <c r="I55" s="349" t="s">
+      <c r="I55" s="350" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="350"/>
-      <c r="K55" s="351">
+      <c r="J55" s="351"/>
+      <c r="K55" s="352">
         <f>F57+F58+F59</f>
         <v>247554.74000000008</v>
       </c>
-      <c r="L55" s="352"/>
+      <c r="L55" s="353"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -13648,11 +13774,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="353">
+      <c r="K57" s="354">
         <f>-C4</f>
         <v>-149938.81</v>
       </c>
-      <c r="L57" s="354"/>
+      <c r="L57" s="355"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -13669,22 +13795,22 @@
       <c r="C59" s="128">
         <v>44745</v>
       </c>
-      <c r="D59" s="330" t="s">
+      <c r="D59" s="331" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="331"/>
+      <c r="E59" s="332"/>
       <c r="F59" s="129">
         <v>232165.91</v>
       </c>
-      <c r="I59" s="332" t="s">
+      <c r="I59" s="333" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="333"/>
-      <c r="K59" s="334">
+      <c r="J59" s="334"/>
+      <c r="K59" s="335">
         <f>K55+K57</f>
         <v>97615.93000000008</v>
       </c>
-      <c r="L59" s="334"/>
+      <c r="L59" s="335"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -15314,23 +15440,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="317"/>
-      <c r="C1" s="319" t="s">
+      <c r="B1" s="318"/>
+      <c r="C1" s="320" t="s">
         <v>380</v>
       </c>
-      <c r="D1" s="320"/>
-      <c r="E1" s="320"/>
-      <c r="F1" s="320"/>
-      <c r="G1" s="320"/>
-      <c r="H1" s="320"/>
-      <c r="I1" s="320"/>
-      <c r="J1" s="320"/>
-      <c r="K1" s="320"/>
-      <c r="L1" s="320"/>
-      <c r="M1" s="320"/>
+      <c r="D1" s="321"/>
+      <c r="E1" s="321"/>
+      <c r="F1" s="321"/>
+      <c r="G1" s="321"/>
+      <c r="H1" s="321"/>
+      <c r="I1" s="321"/>
+      <c r="J1" s="321"/>
+      <c r="K1" s="321"/>
+      <c r="L1" s="321"/>
+      <c r="M1" s="321"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="318"/>
+      <c r="B2" s="319"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -15340,21 +15466,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="321" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="322"/>
+      <c r="B3" s="322" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="323"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="323" t="s">
+      <c r="H3" s="324" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="323"/>
+      <c r="I3" s="324"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="328" t="s">
+      <c r="R3" s="329" t="s">
         <v>38</v>
       </c>
     </row>
@@ -15369,14 +15495,14 @@
       <c r="D4" s="16">
         <v>44745</v>
       </c>
-      <c r="E4" s="324" t="s">
+      <c r="E4" s="325" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="325"/>
-      <c r="H4" s="326" t="s">
+      <c r="F4" s="326"/>
+      <c r="H4" s="327" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="327"/>
+      <c r="I4" s="328"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -15386,11 +15512,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="335" t="s">
+      <c r="P4" s="336" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="336"/>
-      <c r="R4" s="329"/>
+      <c r="Q4" s="337"/>
+      <c r="R4" s="330"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -16835,11 +16961,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="74"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="337">
+      <c r="M40" s="338">
         <f>SUM(M5:M39)</f>
         <v>2373103</v>
       </c>
-      <c r="N40" s="339">
+      <c r="N40" s="340">
         <f>SUM(N5:N39)</f>
         <v>67308</v>
       </c>
@@ -16868,8 +16994,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="235"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="338"/>
-      <c r="N41" s="340"/>
+      <c r="M41" s="339"/>
+      <c r="N41" s="341"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -17084,29 +17210,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="341" t="s">
+      <c r="H53" s="342" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="342"/>
+      <c r="I53" s="343"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="343">
+      <c r="K53" s="344">
         <f>I51+L51</f>
         <v>79649.720000000016</v>
       </c>
-      <c r="L53" s="344"/>
-      <c r="M53" s="345">
+      <c r="L53" s="345"/>
+      <c r="M53" s="346">
         <f>N40+M40</f>
         <v>2440411</v>
       </c>
-      <c r="N53" s="346"/>
+      <c r="N53" s="347"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="347" t="s">
+      <c r="D54" s="348" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="347"/>
+      <c r="E54" s="348"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2356249.2799999998</v>
@@ -17117,22 +17243,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="348" t="s">
+      <c r="D55" s="349" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="348"/>
+      <c r="E55" s="349"/>
       <c r="F55" s="111">
         <v>-2471332.31</v>
       </c>
-      <c r="I55" s="349" t="s">
+      <c r="I55" s="350" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="350"/>
-      <c r="K55" s="351">
+      <c r="J55" s="351"/>
+      <c r="K55" s="352">
         <f>F57+F58+F59</f>
         <v>214026.38999999972</v>
       </c>
-      <c r="L55" s="352"/>
+      <c r="L55" s="353"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -17163,11 +17289,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="353">
+      <c r="K57" s="354">
         <f>-C4</f>
         <v>-232165.91</v>
       </c>
-      <c r="L57" s="354"/>
+      <c r="L57" s="355"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -17184,22 +17310,22 @@
       <c r="C59" s="128">
         <v>44773</v>
       </c>
-      <c r="D59" s="330" t="s">
+      <c r="D59" s="331" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="331"/>
+      <c r="E59" s="332"/>
       <c r="F59" s="129">
         <v>273736.42</v>
       </c>
-      <c r="I59" s="332" t="s">
+      <c r="I59" s="333" t="s">
         <v>325</v>
       </c>
-      <c r="J59" s="333"/>
-      <c r="K59" s="334">
+      <c r="J59" s="334"/>
+      <c r="K59" s="335">
         <f>K55+K57</f>
         <v>-18139.520000000281</v>
       </c>
-      <c r="L59" s="334"/>
+      <c r="L59" s="335"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -18712,7 +18838,7 @@
   </sheetPr>
   <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
@@ -18736,23 +18862,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="317"/>
-      <c r="C1" s="319" t="s">
+      <c r="B1" s="318"/>
+      <c r="C1" s="320" t="s">
         <v>421</v>
       </c>
-      <c r="D1" s="320"/>
-      <c r="E1" s="320"/>
-      <c r="F1" s="320"/>
-      <c r="G1" s="320"/>
-      <c r="H1" s="320"/>
-      <c r="I1" s="320"/>
-      <c r="J1" s="320"/>
-      <c r="K1" s="320"/>
-      <c r="L1" s="320"/>
-      <c r="M1" s="320"/>
+      <c r="D1" s="321"/>
+      <c r="E1" s="321"/>
+      <c r="F1" s="321"/>
+      <c r="G1" s="321"/>
+      <c r="H1" s="321"/>
+      <c r="I1" s="321"/>
+      <c r="J1" s="321"/>
+      <c r="K1" s="321"/>
+      <c r="L1" s="321"/>
+      <c r="M1" s="321"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="318"/>
+      <c r="B2" s="319"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -18762,21 +18888,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="321" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="322"/>
+      <c r="B3" s="322" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="323"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="323" t="s">
+      <c r="H3" s="324" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="323"/>
+      <c r="I3" s="324"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="328" t="s">
+      <c r="R3" s="329" t="s">
         <v>38</v>
       </c>
     </row>
@@ -18791,14 +18917,14 @@
       <c r="D4" s="16">
         <v>44773</v>
       </c>
-      <c r="E4" s="324" t="s">
+      <c r="E4" s="325" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="325"/>
-      <c r="H4" s="326" t="s">
+      <c r="F4" s="326"/>
+      <c r="H4" s="327" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="327"/>
+      <c r="I4" s="328"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -18808,11 +18934,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="335" t="s">
+      <c r="P4" s="336" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="336"/>
-      <c r="R4" s="329"/>
+      <c r="Q4" s="337"/>
+      <c r="R4" s="330"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -20292,11 +20418,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="74"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="337">
+      <c r="M40" s="338">
         <f>SUM(M5:M39)</f>
         <v>2375259</v>
       </c>
-      <c r="N40" s="339">
+      <c r="N40" s="340">
         <f>SUM(N5:N39)</f>
         <v>61117</v>
       </c>
@@ -20325,8 +20451,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="235"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="338"/>
-      <c r="N41" s="340"/>
+      <c r="M41" s="339"/>
+      <c r="N41" s="341"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -20541,29 +20667,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="341" t="s">
+      <c r="H53" s="342" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="342"/>
+      <c r="I53" s="343"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="343">
+      <c r="K53" s="344">
         <f>I51+L51</f>
         <v>52857.25</v>
       </c>
-      <c r="L53" s="344"/>
-      <c r="M53" s="345">
+      <c r="L53" s="345"/>
+      <c r="M53" s="346">
         <f>N40+M40</f>
         <v>2436376</v>
       </c>
-      <c r="N53" s="346"/>
+      <c r="N53" s="347"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="347" t="s">
+      <c r="D54" s="348" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="347"/>
+      <c r="E54" s="348"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2370653.75</v>
@@ -20574,22 +20700,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="348" t="s">
+      <c r="D55" s="349" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="348"/>
+      <c r="E55" s="349"/>
       <c r="F55" s="111">
         <v>-2401197.5699999998</v>
       </c>
-      <c r="I55" s="349" t="s">
+      <c r="I55" s="350" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="350"/>
-      <c r="K55" s="351">
+      <c r="J55" s="351"/>
+      <c r="K55" s="352">
         <f>F57+F58+F59</f>
         <v>259241.77000000016</v>
       </c>
-      <c r="L55" s="352"/>
+      <c r="L55" s="353"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -20620,11 +20746,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="353">
+      <c r="K57" s="354">
         <f>-C4</f>
         <v>-273736.42</v>
       </c>
-      <c r="L57" s="354"/>
+      <c r="L57" s="355"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -20641,22 +20767,22 @@
       <c r="C59" s="128">
         <v>44801</v>
       </c>
-      <c r="D59" s="330" t="s">
+      <c r="D59" s="331" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="331"/>
+      <c r="E59" s="332"/>
       <c r="F59" s="129">
         <v>236400.59</v>
       </c>
-      <c r="I59" s="356" t="s">
+      <c r="I59" s="357" t="s">
         <v>325</v>
       </c>
-      <c r="J59" s="357"/>
-      <c r="K59" s="358">
+      <c r="J59" s="358"/>
+      <c r="K59" s="359">
         <f>K55+K57</f>
         <v>-14494.64999999982</v>
       </c>
-      <c r="L59" s="358"/>
+      <c r="L59" s="359"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -22180,10 +22306,10 @@
   <dimension ref="A1:U81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="E29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I44" sqref="I44"/>
+      <selection pane="bottomRight" activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22208,23 +22334,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="317"/>
-      <c r="C1" s="319" t="s">
+      <c r="B1" s="318"/>
+      <c r="C1" s="320" t="s">
         <v>465</v>
       </c>
-      <c r="D1" s="320"/>
-      <c r="E1" s="320"/>
-      <c r="F1" s="320"/>
-      <c r="G1" s="320"/>
-      <c r="H1" s="320"/>
-      <c r="I1" s="320"/>
-      <c r="J1" s="320"/>
-      <c r="K1" s="320"/>
-      <c r="L1" s="320"/>
-      <c r="M1" s="320"/>
+      <c r="D1" s="321"/>
+      <c r="E1" s="321"/>
+      <c r="F1" s="321"/>
+      <c r="G1" s="321"/>
+      <c r="H1" s="321"/>
+      <c r="I1" s="321"/>
+      <c r="J1" s="321"/>
+      <c r="K1" s="321"/>
+      <c r="L1" s="321"/>
+      <c r="M1" s="321"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="318"/>
+      <c r="B2" s="319"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -22234,21 +22360,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="321" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="322"/>
+      <c r="B3" s="322" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="323"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="323" t="s">
+      <c r="H3" s="324" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="323"/>
+      <c r="I3" s="324"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="328" t="s">
+      <c r="R3" s="329" t="s">
         <v>38</v>
       </c>
     </row>
@@ -22263,14 +22389,14 @@
       <c r="D4" s="16">
         <v>44801</v>
       </c>
-      <c r="E4" s="324" t="s">
+      <c r="E4" s="325" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="325"/>
-      <c r="H4" s="326" t="s">
+      <c r="F4" s="326"/>
+      <c r="H4" s="327" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="327"/>
+      <c r="I4" s="328"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -22280,11 +22406,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="335" t="s">
+      <c r="P4" s="336" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="336"/>
-      <c r="R4" s="329"/>
+      <c r="Q4" s="337"/>
+      <c r="R4" s="330"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -23949,30 +24075,37 @@
         <v>44836</v>
       </c>
       <c r="C39" s="24">
-        <v>0</v>
-      </c>
-      <c r="D39" s="77"/>
+        <v>16</v>
+      </c>
+      <c r="D39" s="77" t="s">
+        <v>34</v>
+      </c>
       <c r="E39" s="26">
         <v>44836</v>
       </c>
-      <c r="F39" s="83"/>
+      <c r="F39" s="83">
+        <v>145363</v>
+      </c>
       <c r="H39" s="28">
         <v>44836</v>
       </c>
-      <c r="I39" s="29"/>
+      <c r="I39" s="29">
+        <v>70</v>
+      </c>
       <c r="J39" s="71"/>
       <c r="K39" s="266"/>
       <c r="L39" s="73"/>
       <c r="M39" s="30">
-        <v>0</v>
+        <f>16456+85000+40000</f>
+        <v>141456</v>
       </c>
       <c r="N39" s="31">
-        <v>0</v>
+        <v>3821</v>
       </c>
       <c r="O39" s="314"/>
       <c r="P39" s="32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>145363</v>
       </c>
       <c r="Q39" s="12">
         <f t="shared" si="1"/>
@@ -23996,20 +24129,26 @@
       <c r="F40" s="85"/>
       <c r="H40" s="28"/>
       <c r="I40" s="86"/>
-      <c r="J40" s="71"/>
-      <c r="K40" s="74"/>
-      <c r="L40" s="73"/>
-      <c r="M40" s="337">
+      <c r="J40" s="71">
+        <v>44804</v>
+      </c>
+      <c r="K40" s="317" t="s">
+        <v>204</v>
+      </c>
+      <c r="L40" s="73">
+        <v>927.48</v>
+      </c>
+      <c r="M40" s="338">
         <f>SUM(M5:M39)</f>
-        <v>3005853.5</v>
-      </c>
-      <c r="N40" s="339">
+        <v>3147309.5</v>
+      </c>
+      <c r="N40" s="340">
         <f>SUM(N5:N39)</f>
-        <v>72748</v>
+        <v>76569</v>
       </c>
       <c r="P40" s="32">
         <f t="shared" si="0"/>
-        <v>3078601.5</v>
+        <v>3224805.98</v>
       </c>
       <c r="Q40" s="284">
         <f>SUM(Q5:Q39)</f>
@@ -24029,11 +24168,17 @@
       <c r="F41" s="249"/>
       <c r="H41" s="250"/>
       <c r="I41" s="86"/>
-      <c r="J41" s="71"/>
-      <c r="K41" s="235"/>
-      <c r="L41" s="73"/>
-      <c r="M41" s="338"/>
-      <c r="N41" s="340"/>
+      <c r="J41" s="71">
+        <v>44809</v>
+      </c>
+      <c r="K41" s="360" t="s">
+        <v>190</v>
+      </c>
+      <c r="L41" s="73">
+        <v>33312</v>
+      </c>
+      <c r="M41" s="339"/>
+      <c r="N41" s="341"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -24049,9 +24194,15 @@
       <c r="I42" s="93" t="s">
         <v>471</v>
       </c>
-      <c r="J42" s="71"/>
-      <c r="K42" s="74"/>
-      <c r="L42" s="78"/>
+      <c r="J42" s="71">
+        <v>44814</v>
+      </c>
+      <c r="K42" s="235" t="s">
+        <v>205</v>
+      </c>
+      <c r="L42" s="73">
+        <v>1392</v>
+      </c>
       <c r="M42" s="94"/>
       <c r="N42" s="95"/>
       <c r="P42" s="32"/>
@@ -24067,9 +24218,15 @@
       <c r="G43" s="251"/>
       <c r="H43" s="35"/>
       <c r="I43" s="93"/>
-      <c r="J43" s="71"/>
-      <c r="K43" s="74"/>
-      <c r="L43" s="78"/>
+      <c r="J43" s="71">
+        <v>44824</v>
+      </c>
+      <c r="K43" s="74" t="s">
+        <v>464</v>
+      </c>
+      <c r="L43" s="78">
+        <v>549</v>
+      </c>
       <c r="M43" s="94"/>
       <c r="N43" s="95"/>
       <c r="P43" s="32"/>
@@ -24084,10 +24241,18 @@
       <c r="F44" s="235"/>
       <c r="G44" s="251"/>
       <c r="H44" s="35"/>
-      <c r="I44" s="93"/>
-      <c r="J44" s="71"/>
-      <c r="K44" s="132"/>
-      <c r="L44" s="78"/>
+      <c r="I44" s="93" t="s">
+        <v>473</v>
+      </c>
+      <c r="J44" s="71">
+        <v>44830</v>
+      </c>
+      <c r="K44" s="361" t="s">
+        <v>204</v>
+      </c>
+      <c r="L44" s="78">
+        <v>979.68</v>
+      </c>
       <c r="M44" s="94"/>
       <c r="N44" s="95"/>
       <c r="P44" s="32"/>
@@ -24103,9 +24268,15 @@
       <c r="G45" s="251"/>
       <c r="H45" s="35"/>
       <c r="I45" s="93"/>
-      <c r="J45" s="71"/>
-      <c r="K45" s="74"/>
-      <c r="L45" s="78"/>
+      <c r="J45" s="71">
+        <v>44834</v>
+      </c>
+      <c r="K45" s="74" t="s">
+        <v>378</v>
+      </c>
+      <c r="L45" s="78">
+        <v>3257.71</v>
+      </c>
       <c r="M45" s="94"/>
       <c r="N45" s="95"/>
       <c r="P45" s="32"/>
@@ -24208,7 +24379,7 @@
       </c>
       <c r="C51" s="102">
         <f>SUM(C5:C50)</f>
-        <v>131688</v>
+        <v>131704</v>
       </c>
       <c r="D51" s="103"/>
       <c r="E51" s="104" t="s">
@@ -24216,7 +24387,7 @@
       </c>
       <c r="F51" s="105">
         <f>SUM(F5:F50)</f>
-        <v>3219291</v>
+        <v>3364654</v>
       </c>
       <c r="G51" s="103"/>
       <c r="H51" s="106" t="s">
@@ -24224,7 +24395,7 @@
       </c>
       <c r="I51" s="107">
         <f>SUM(I5:I50)</f>
-        <v>5182</v>
+        <v>5252</v>
       </c>
       <c r="J51" s="108"/>
       <c r="K51" s="109" t="s">
@@ -24232,7 +24403,7 @@
       </c>
       <c r="L51" s="110">
         <f>SUM(L5:L50)</f>
-        <v>57204</v>
+        <v>97621.87000000001</v>
       </c>
       <c r="M51" s="111"/>
       <c r="N51" s="111"/>
@@ -24250,32 +24421,32 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="341" t="s">
+      <c r="H53" s="342" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="342"/>
+      <c r="I53" s="343"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="343">
+      <c r="K53" s="344">
         <f>I51+L51</f>
-        <v>62386</v>
-      </c>
-      <c r="L53" s="344"/>
-      <c r="M53" s="345">
+        <v>102873.87000000001</v>
+      </c>
+      <c r="L53" s="345"/>
+      <c r="M53" s="346">
         <f>N40+M40</f>
-        <v>3078601.5</v>
-      </c>
-      <c r="N53" s="346"/>
+        <v>3223878.5</v>
+      </c>
+      <c r="N53" s="347"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="347" t="s">
+      <c r="D54" s="348" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="347"/>
+      <c r="E54" s="348"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
-        <v>3025217</v>
+        <v>3130076.13</v>
       </c>
       <c r="I54" s="116"/>
       <c r="J54" s="117"/>
@@ -24283,22 +24454,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="348" t="s">
+      <c r="D55" s="349" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="348"/>
+      <c r="E55" s="349"/>
       <c r="F55" s="111">
-        <v>0</v>
-      </c>
-      <c r="I55" s="349" t="s">
+        <v>-3171951.31</v>
+      </c>
+      <c r="I55" s="350" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="350"/>
-      <c r="K55" s="351">
+      <c r="J55" s="351"/>
+      <c r="K55" s="352">
         <f>F57+F58+F59</f>
-        <v>3025217</v>
-      </c>
-      <c r="L55" s="352"/>
+        <v>265314.0299999998</v>
+      </c>
+      <c r="L55" s="353"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -24322,18 +24493,18 @@
       </c>
       <c r="F57" s="111">
         <f>SUM(F54:F56)</f>
-        <v>3025217</v>
+        <v>-41875.180000000168</v>
       </c>
       <c r="H57" s="22"/>
       <c r="I57" s="124" t="s">
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="353">
+      <c r="K57" s="354">
         <f>-C4</f>
         <v>-236400.59</v>
       </c>
-      <c r="L57" s="354"/>
+      <c r="L57" s="355"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -24343,27 +24514,29 @@
         <v>19</v>
       </c>
       <c r="F58" s="127">
-        <v>0</v>
+        <v>64835</v>
       </c>
     </row>
     <row r="59" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C59" s="128"/>
-      <c r="D59" s="330" t="s">
+      <c r="C59" s="128">
+        <v>44836</v>
+      </c>
+      <c r="D59" s="331" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="331"/>
+      <c r="E59" s="332"/>
       <c r="F59" s="129">
-        <v>0</v>
-      </c>
-      <c r="I59" s="356" t="s">
+        <v>242354.21</v>
+      </c>
+      <c r="I59" s="357" t="s">
         <v>325</v>
       </c>
-      <c r="J59" s="357"/>
-      <c r="K59" s="358">
+      <c r="J59" s="358"/>
+      <c r="K59" s="359">
         <f>K55+K57</f>
-        <v>2788816.41</v>
-      </c>
-      <c r="L59" s="358"/>
+        <v>28913.439999999799</v>
+      </c>
+      <c r="L59" s="359"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -24487,6 +24660,9 @@
       <c r="F81" s="144"/>
     </row>
   </sheetData>
+  <sortState ref="J41:L45">
+    <sortCondition ref="J41:J45"/>
+  </sortState>
   <mergeCells count="21">
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
@@ -24524,8 +24700,8 @@
   </sheetPr>
   <dimension ref="A1:J115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24574,113 +24750,167 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="254"/>
-      <c r="B3" s="255"/>
-      <c r="C3" s="256"/>
+      <c r="A3" s="254">
+        <v>44802</v>
+      </c>
+      <c r="B3" s="255" t="s">
+        <v>474</v>
+      </c>
+      <c r="C3" s="256">
+        <v>121359.44</v>
+      </c>
       <c r="D3" s="302"/>
       <c r="E3" s="303"/>
       <c r="F3" s="152">
         <f>C3-E3</f>
-        <v>0</v>
+        <v>121359.44</v>
       </c>
       <c r="J3" s="127"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="257"/>
-      <c r="B4" s="258"/>
-      <c r="C4" s="127"/>
+      <c r="A4" s="257">
+        <v>44804</v>
+      </c>
+      <c r="B4" s="258" t="s">
+        <v>475</v>
+      </c>
+      <c r="C4" s="127">
+        <v>70490.48</v>
+      </c>
       <c r="D4" s="302"/>
       <c r="E4" s="294"/>
       <c r="F4" s="188">
         <f>C4-E4+F3</f>
-        <v>0</v>
+        <v>191849.91999999998</v>
       </c>
       <c r="J4" s="256"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="257"/>
-      <c r="B5" s="258"/>
-      <c r="C5" s="127"/>
+      <c r="A5" s="257">
+        <v>44805</v>
+      </c>
+      <c r="B5" s="258" t="s">
+        <v>476</v>
+      </c>
+      <c r="C5" s="127">
+        <v>9687.1</v>
+      </c>
       <c r="D5" s="302"/>
       <c r="E5" s="294"/>
       <c r="F5" s="188">
         <f t="shared" ref="F5:F68" si="0">C5-E5+F4</f>
-        <v>0</v>
+        <v>201537.02</v>
       </c>
       <c r="J5" s="127"/>
     </row>
     <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="257"/>
-      <c r="B6" s="258"/>
-      <c r="C6" s="127"/>
+      <c r="A6" s="257">
+        <v>44805</v>
+      </c>
+      <c r="B6" s="258" t="s">
+        <v>477</v>
+      </c>
+      <c r="C6" s="127">
+        <v>1392.3</v>
+      </c>
       <c r="D6" s="302"/>
       <c r="E6" s="294"/>
       <c r="F6" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>202929.31999999998</v>
       </c>
       <c r="G6" s="156"/>
       <c r="J6" s="127"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="257"/>
-      <c r="B7" s="258"/>
-      <c r="C7" s="127"/>
+      <c r="A7" s="257">
+        <v>44805</v>
+      </c>
+      <c r="B7" s="258" t="s">
+        <v>478</v>
+      </c>
+      <c r="C7" s="127">
+        <v>63143.99</v>
+      </c>
       <c r="D7" s="302"/>
       <c r="E7" s="294"/>
       <c r="F7" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>266073.31</v>
       </c>
       <c r="J7" s="127"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="257"/>
-      <c r="B8" s="258"/>
-      <c r="C8" s="127"/>
+      <c r="A8" s="257">
+        <v>44806</v>
+      </c>
+      <c r="B8" s="258" t="s">
+        <v>479</v>
+      </c>
+      <c r="C8" s="127">
+        <v>110657.18</v>
+      </c>
       <c r="D8" s="302"/>
       <c r="E8" s="294"/>
       <c r="F8" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>376730.49</v>
       </c>
       <c r="J8" s="127"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="257"/>
-      <c r="B9" s="258"/>
-      <c r="C9" s="127"/>
+      <c r="A9" s="257">
+        <v>44806</v>
+      </c>
+      <c r="B9" s="258" t="s">
+        <v>480</v>
+      </c>
+      <c r="C9" s="127">
+        <v>20028.400000000001</v>
+      </c>
       <c r="D9" s="276"/>
       <c r="E9" s="277"/>
       <c r="F9" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>396758.89</v>
       </c>
       <c r="J9" s="127"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="257"/>
-      <c r="B10" s="258"/>
-      <c r="C10" s="127"/>
+      <c r="A10" s="257">
+        <v>44807</v>
+      </c>
+      <c r="B10" s="258" t="s">
+        <v>481</v>
+      </c>
+      <c r="C10" s="127">
+        <v>99866.84</v>
+      </c>
       <c r="D10" s="276"/>
       <c r="E10" s="277"/>
       <c r="F10" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>496625.73</v>
       </c>
       <c r="J10" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="257"/>
-      <c r="B11" s="258"/>
-      <c r="C11" s="127"/>
+      <c r="A11" s="257">
+        <v>44808</v>
+      </c>
+      <c r="B11" s="258" t="s">
+        <v>482</v>
+      </c>
+      <c r="C11" s="127">
+        <v>4343</v>
+      </c>
       <c r="D11" s="276"/>
       <c r="E11" s="277"/>
       <c r="F11" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>500968.73</v>
       </c>
       <c r="J11" s="267">
         <f>SUM(J3:J10)</f>
@@ -24688,325 +24918,499 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="257"/>
-      <c r="B12" s="258"/>
-      <c r="C12" s="127"/>
+      <c r="A12" s="257">
+        <v>44809</v>
+      </c>
+      <c r="B12" s="258" t="s">
+        <v>483</v>
+      </c>
+      <c r="C12" s="127">
+        <v>162404.20000000001</v>
+      </c>
       <c r="D12" s="276"/>
       <c r="E12" s="277"/>
       <c r="F12" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>663372.92999999993</v>
       </c>
       <c r="G12" s="156"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="257"/>
-      <c r="B13" s="258"/>
-      <c r="C13" s="127"/>
+      <c r="A13" s="257">
+        <v>44810</v>
+      </c>
+      <c r="B13" s="258" t="s">
+        <v>484</v>
+      </c>
+      <c r="C13" s="127">
+        <v>100681.72</v>
+      </c>
       <c r="D13" s="276"/>
       <c r="E13" s="277"/>
       <c r="F13" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>764054.64999999991</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="257"/>
-      <c r="B14" s="258"/>
-      <c r="C14" s="127"/>
+      <c r="A14" s="257">
+        <v>44810</v>
+      </c>
+      <c r="B14" s="258" t="s">
+        <v>485</v>
+      </c>
+      <c r="C14" s="127">
+        <v>4737.7</v>
+      </c>
       <c r="D14" s="276"/>
       <c r="E14" s="277"/>
       <c r="F14" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>768792.34999999986</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="257"/>
-      <c r="B15" s="258"/>
-      <c r="C15" s="127"/>
+      <c r="A15" s="257">
+        <v>44812</v>
+      </c>
+      <c r="B15" s="258" t="s">
+        <v>486</v>
+      </c>
+      <c r="C15" s="127">
+        <v>126371.9</v>
+      </c>
       <c r="D15" s="276"/>
       <c r="E15" s="277"/>
       <c r="F15" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>895164.24999999988</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="257"/>
-      <c r="B16" s="258"/>
-      <c r="C16" s="127"/>
+      <c r="A16" s="257">
+        <v>44814</v>
+      </c>
+      <c r="B16" s="258" t="s">
+        <v>487</v>
+      </c>
+      <c r="C16" s="127">
+        <v>151423.09</v>
+      </c>
       <c r="D16" s="276"/>
       <c r="E16" s="277"/>
       <c r="F16" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1046587.3399999999</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="257"/>
-      <c r="B17" s="258"/>
-      <c r="C17" s="127"/>
+      <c r="A17" s="257">
+        <v>44814</v>
+      </c>
+      <c r="B17" s="258" t="s">
+        <v>488</v>
+      </c>
+      <c r="C17" s="127">
+        <v>2880</v>
+      </c>
       <c r="D17" s="276"/>
       <c r="E17" s="277"/>
       <c r="F17" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1049467.3399999999</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="257"/>
-      <c r="B18" s="258"/>
-      <c r="C18" s="127"/>
+      <c r="A18" s="257">
+        <v>44815</v>
+      </c>
+      <c r="B18" s="258" t="s">
+        <v>489</v>
+      </c>
+      <c r="C18" s="127">
+        <v>43875.1</v>
+      </c>
       <c r="D18" s="304"/>
       <c r="E18" s="274"/>
       <c r="F18" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1093342.44</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="257"/>
-      <c r="B19" s="258"/>
-      <c r="C19" s="127"/>
+      <c r="A19" s="257">
+        <v>44816</v>
+      </c>
+      <c r="B19" s="258" t="s">
+        <v>490</v>
+      </c>
+      <c r="C19" s="127">
+        <v>130202.7</v>
+      </c>
       <c r="D19" s="304"/>
       <c r="E19" s="274"/>
       <c r="F19" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1223545.1399999999</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="257"/>
-      <c r="B20" s="258"/>
-      <c r="C20" s="127"/>
+      <c r="A20" s="257">
+        <v>44817</v>
+      </c>
+      <c r="B20" s="258" t="s">
+        <v>491</v>
+      </c>
+      <c r="C20" s="127">
+        <v>143921.60000000001</v>
+      </c>
       <c r="D20" s="304"/>
       <c r="E20" s="274"/>
       <c r="F20" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1367466.74</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="257"/>
-      <c r="B21" s="258"/>
-      <c r="C21" s="127"/>
+      <c r="A21" s="257">
+        <v>44818</v>
+      </c>
+      <c r="B21" s="258" t="s">
+        <v>492</v>
+      </c>
+      <c r="C21" s="127">
+        <v>134490</v>
+      </c>
       <c r="D21" s="304"/>
       <c r="E21" s="274"/>
       <c r="F21" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1501956.74</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="257"/>
-      <c r="B22" s="258"/>
-      <c r="C22" s="127"/>
+      <c r="A22" s="257">
+        <v>44819</v>
+      </c>
+      <c r="B22" s="258" t="s">
+        <v>493</v>
+      </c>
+      <c r="C22" s="127">
+        <v>15710.72</v>
+      </c>
       <c r="D22" s="304"/>
       <c r="E22" s="274"/>
       <c r="F22" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1517667.46</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="257"/>
-      <c r="B23" s="258"/>
-      <c r="C23" s="127"/>
+      <c r="A23" s="257">
+        <v>44820</v>
+      </c>
+      <c r="B23" s="258" t="s">
+        <v>494</v>
+      </c>
+      <c r="C23" s="127">
+        <v>145559.48000000001</v>
+      </c>
       <c r="D23" s="304"/>
       <c r="E23" s="274"/>
       <c r="F23" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1663226.94</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="257"/>
-      <c r="B24" s="258"/>
-      <c r="C24" s="127"/>
+      <c r="A24" s="257">
+        <v>44821</v>
+      </c>
+      <c r="B24" s="258" t="s">
+        <v>495</v>
+      </c>
+      <c r="C24" s="127">
+        <v>43231.199999999997</v>
+      </c>
       <c r="D24" s="304"/>
       <c r="E24" s="274"/>
       <c r="F24" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1706458.14</v>
       </c>
       <c r="G24" s="156"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="257"/>
-      <c r="B25" s="258"/>
-      <c r="C25" s="127"/>
+      <c r="A25" s="257">
+        <v>44821</v>
+      </c>
+      <c r="B25" s="258" t="s">
+        <v>496</v>
+      </c>
+      <c r="C25" s="127">
+        <v>74093.38</v>
+      </c>
       <c r="D25" s="304"/>
       <c r="E25" s="274"/>
       <c r="F25" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1780551.52</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="257"/>
-      <c r="B26" s="258"/>
-      <c r="C26" s="127"/>
+      <c r="A26" s="257">
+        <v>44821</v>
+      </c>
+      <c r="B26" s="258" t="s">
+        <v>497</v>
+      </c>
+      <c r="C26" s="127">
+        <v>1852.32</v>
+      </c>
       <c r="D26" s="259"/>
       <c r="E26" s="127"/>
       <c r="F26" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1782403.84</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="257"/>
-      <c r="B27" s="258"/>
-      <c r="C27" s="127"/>
+      <c r="A27" s="257">
+        <v>44821</v>
+      </c>
+      <c r="B27" s="258" t="s">
+        <v>498</v>
+      </c>
+      <c r="C27" s="127">
+        <v>15179.4</v>
+      </c>
       <c r="D27" s="259"/>
       <c r="E27" s="127"/>
       <c r="F27" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1797583.24</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="257"/>
-      <c r="B28" s="258"/>
-      <c r="C28" s="127"/>
+      <c r="A28" s="257">
+        <v>44822</v>
+      </c>
+      <c r="B28" s="258" t="s">
+        <v>499</v>
+      </c>
+      <c r="C28" s="127">
+        <v>78457.2</v>
+      </c>
       <c r="D28" s="259"/>
       <c r="E28" s="127"/>
       <c r="F28" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1876040.44</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="257"/>
-      <c r="B29" s="258"/>
-      <c r="C29" s="127"/>
+      <c r="A29" s="257">
+        <v>44823</v>
+      </c>
+      <c r="B29" s="258" t="s">
+        <v>500</v>
+      </c>
+      <c r="C29" s="127">
+        <v>72034.820000000007</v>
+      </c>
       <c r="D29" s="259"/>
       <c r="E29" s="127"/>
       <c r="F29" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1948075.26</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="257"/>
-      <c r="B30" s="258"/>
-      <c r="C30" s="127"/>
+      <c r="A30" s="257">
+        <v>44824</v>
+      </c>
+      <c r="B30" s="258" t="s">
+        <v>501</v>
+      </c>
+      <c r="C30" s="127">
+        <v>150680.32000000001</v>
+      </c>
       <c r="D30" s="257"/>
       <c r="E30" s="127"/>
       <c r="F30" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2098755.58</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="257"/>
-      <c r="B31" s="258"/>
-      <c r="C31" s="127"/>
+      <c r="A31" s="257">
+        <v>44825</v>
+      </c>
+      <c r="B31" s="258" t="s">
+        <v>502</v>
+      </c>
+      <c r="C31" s="127">
+        <v>168795.67</v>
+      </c>
       <c r="D31" s="259"/>
       <c r="E31" s="127"/>
       <c r="F31" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2267551.25</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="257"/>
-      <c r="B32" s="258"/>
-      <c r="C32" s="127"/>
+      <c r="A32" s="257">
+        <v>44827</v>
+      </c>
+      <c r="B32" s="258" t="s">
+        <v>503</v>
+      </c>
+      <c r="C32" s="127">
+        <v>167099.1</v>
+      </c>
       <c r="D32" s="259"/>
       <c r="E32" s="127"/>
       <c r="F32" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2434650.35</v>
       </c>
       <c r="G32" s="156"/>
     </row>
     <row r="33" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="257"/>
-      <c r="B33" s="258"/>
-      <c r="C33" s="127"/>
+      <c r="A33" s="257">
+        <v>44827</v>
+      </c>
+      <c r="B33" s="258" t="s">
+        <v>504</v>
+      </c>
+      <c r="C33" s="127">
+        <v>10374.799999999999</v>
+      </c>
       <c r="D33" s="259"/>
       <c r="E33" s="127"/>
       <c r="F33" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2445025.15</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="257"/>
-      <c r="B34" s="258"/>
-      <c r="C34" s="127"/>
+      <c r="A34" s="257">
+        <v>44828</v>
+      </c>
+      <c r="B34" s="258" t="s">
+        <v>505</v>
+      </c>
+      <c r="C34" s="127">
+        <v>99260.84</v>
+      </c>
       <c r="D34" s="259"/>
       <c r="E34" s="127"/>
       <c r="F34" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2544285.9899999998</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="257"/>
-      <c r="B35" s="258"/>
-      <c r="C35" s="127"/>
+      <c r="A35" s="257">
+        <v>44830</v>
+      </c>
+      <c r="B35" s="258" t="s">
+        <v>506</v>
+      </c>
+      <c r="C35" s="127">
+        <v>104477.42</v>
+      </c>
       <c r="D35" s="259"/>
       <c r="E35" s="127"/>
       <c r="F35" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2648763.4099999997</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="257"/>
-      <c r="B36" s="258"/>
-      <c r="C36" s="127"/>
+      <c r="A36" s="257">
+        <v>44831</v>
+      </c>
+      <c r="B36" s="258" t="s">
+        <v>507</v>
+      </c>
+      <c r="C36" s="127">
+        <v>74115.039999999994</v>
+      </c>
       <c r="D36" s="259"/>
       <c r="E36" s="127"/>
       <c r="F36" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2722878.4499999997</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="257"/>
-      <c r="B37" s="258"/>
-      <c r="C37" s="127"/>
+      <c r="A37" s="257">
+        <v>44832</v>
+      </c>
+      <c r="B37" s="258" t="s">
+        <v>508</v>
+      </c>
+      <c r="C37" s="127">
+        <v>120675.35</v>
+      </c>
       <c r="D37" s="259"/>
       <c r="E37" s="127"/>
       <c r="F37" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2843553.8</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="257"/>
-      <c r="B38" s="258"/>
-      <c r="C38" s="127"/>
+      <c r="A38" s="257">
+        <v>44833</v>
+      </c>
+      <c r="B38" s="258" t="s">
+        <v>509</v>
+      </c>
+      <c r="C38" s="127">
+        <v>36344.76</v>
+      </c>
       <c r="D38" s="259"/>
       <c r="E38" s="127"/>
       <c r="F38" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2879898.5599999996</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="257"/>
-      <c r="B39" s="258"/>
-      <c r="C39" s="127"/>
+      <c r="A39" s="257">
+        <v>44834</v>
+      </c>
+      <c r="B39" s="258" t="s">
+        <v>510</v>
+      </c>
+      <c r="C39" s="127">
+        <v>171098.38</v>
+      </c>
       <c r="D39" s="259"/>
       <c r="E39" s="127"/>
       <c r="F39" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3050996.9399999995</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="257"/>
-      <c r="B40" s="258"/>
-      <c r="C40" s="127"/>
+      <c r="A40" s="257">
+        <v>44835</v>
+      </c>
+      <c r="B40" s="258" t="s">
+        <v>511</v>
+      </c>
+      <c r="C40" s="127">
+        <v>120954.27</v>
+      </c>
       <c r="D40" s="259"/>
       <c r="E40" s="84"/>
       <c r="F40" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -25017,7 +25421,7 @@
       <c r="E41" s="84"/>
       <c r="F41" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -25028,7 +25432,7 @@
       <c r="E42" s="84"/>
       <c r="F42" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -25039,7 +25443,7 @@
       <c r="E43" s="84"/>
       <c r="F43" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -25050,7 +25454,7 @@
       <c r="E44" s="84"/>
       <c r="F44" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25061,7 +25465,7 @@
       <c r="E45" s="84"/>
       <c r="F45" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25072,7 +25476,7 @@
       <c r="E46" s="84"/>
       <c r="F46" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25083,7 +25487,7 @@
       <c r="E47" s="84"/>
       <c r="F47" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25094,7 +25498,7 @@
       <c r="E48" s="84"/>
       <c r="F48" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25105,7 +25509,7 @@
       <c r="E49" s="84"/>
       <c r="F49" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25116,7 +25520,7 @@
       <c r="E50" s="84"/>
       <c r="F50" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25127,7 +25531,7 @@
       <c r="E51" s="84"/>
       <c r="F51" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25138,7 +25542,7 @@
       <c r="E52" s="84"/>
       <c r="F52" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25149,7 +25553,7 @@
       <c r="E53" s="84"/>
       <c r="F53" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25160,7 +25564,7 @@
       <c r="E54" s="84"/>
       <c r="F54" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25171,7 +25575,7 @@
       <c r="E55" s="84"/>
       <c r="F55" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25182,7 +25586,7 @@
       <c r="E56" s="84"/>
       <c r="F56" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25193,7 +25597,7 @@
       <c r="E57" s="84"/>
       <c r="F57" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25204,7 +25608,7 @@
       <c r="E58" s="84"/>
       <c r="F58" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25215,7 +25619,7 @@
       <c r="E59" s="84"/>
       <c r="F59" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25226,7 +25630,7 @@
       <c r="E60" s="84"/>
       <c r="F60" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25237,7 +25641,7 @@
       <c r="E61" s="84"/>
       <c r="F61" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25248,7 +25652,7 @@
       <c r="E62" s="32"/>
       <c r="F62" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25259,7 +25663,7 @@
       <c r="E63" s="32"/>
       <c r="F63" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25270,7 +25674,7 @@
       <c r="E64" s="32"/>
       <c r="F64" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25281,7 +25685,7 @@
       <c r="E65" s="32"/>
       <c r="F65" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25292,7 +25696,7 @@
       <c r="E66" s="32"/>
       <c r="F66" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25303,7 +25707,7 @@
       <c r="E67" s="32"/>
       <c r="F67" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25314,7 +25718,7 @@
       <c r="E68" s="84"/>
       <c r="F68" s="188">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25325,7 +25729,7 @@
       <c r="E69" s="84"/>
       <c r="F69" s="188">
         <f t="shared" ref="F69:F78" si="1">C69-E69+F68</f>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25336,7 +25740,7 @@
       <c r="E70" s="84"/>
       <c r="F70" s="188">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25347,7 +25751,7 @@
       <c r="E71" s="84"/>
       <c r="F71" s="188">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25358,7 +25762,7 @@
       <c r="E72" s="84"/>
       <c r="F72" s="188">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25369,7 +25773,7 @@
       <c r="E73" s="84"/>
       <c r="F73" s="188">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25380,7 +25784,7 @@
       <c r="E74" s="84"/>
       <c r="F74" s="188">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25391,7 +25795,7 @@
       <c r="E75" s="84"/>
       <c r="F75" s="188">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25402,7 +25806,7 @@
       <c r="E76" s="84"/>
       <c r="F76" s="188">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25413,7 +25817,7 @@
       <c r="E77" s="84"/>
       <c r="F77" s="188">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -25426,7 +25830,7 @@
       <c r="E78" s="32"/>
       <c r="F78" s="188">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -25434,7 +25838,7 @@
       <c r="B79" s="223"/>
       <c r="C79" s="240">
         <f>SUM(C3:C78)</f>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
       <c r="D79" s="181"/>
       <c r="E79" s="170">
@@ -25443,7 +25847,7 @@
       </c>
       <c r="F79" s="171">
         <f>F78</f>
-        <v>0</v>
+        <v>3171951.2099999995</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -27410,23 +27814,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="317"/>
-      <c r="C1" s="319" t="s">
+      <c r="B1" s="318"/>
+      <c r="C1" s="320" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="320"/>
-      <c r="E1" s="320"/>
-      <c r="F1" s="320"/>
-      <c r="G1" s="320"/>
-      <c r="H1" s="320"/>
-      <c r="I1" s="320"/>
-      <c r="J1" s="320"/>
-      <c r="K1" s="320"/>
-      <c r="L1" s="320"/>
-      <c r="M1" s="320"/>
+      <c r="D1" s="321"/>
+      <c r="E1" s="321"/>
+      <c r="F1" s="321"/>
+      <c r="G1" s="321"/>
+      <c r="H1" s="321"/>
+      <c r="I1" s="321"/>
+      <c r="J1" s="321"/>
+      <c r="K1" s="321"/>
+      <c r="L1" s="321"/>
+      <c r="M1" s="321"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="318"/>
+      <c r="B2" s="319"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -27436,21 +27840,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="321" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="322"/>
+      <c r="B3" s="322" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="323"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="323" t="s">
+      <c r="H3" s="324" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="323"/>
+      <c r="I3" s="324"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="328" t="s">
+      <c r="R3" s="329" t="s">
         <v>38</v>
       </c>
     </row>
@@ -27465,14 +27869,14 @@
       <c r="D4" s="16">
         <v>44591</v>
       </c>
-      <c r="E4" s="324" t="s">
+      <c r="E4" s="325" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="325"/>
-      <c r="H4" s="326" t="s">
+      <c r="F4" s="326"/>
+      <c r="H4" s="327" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="327"/>
+      <c r="I4" s="328"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -27482,11 +27886,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="335" t="s">
+      <c r="P4" s="336" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="336"/>
-      <c r="R4" s="329"/>
+      <c r="Q4" s="337"/>
+      <c r="R4" s="330"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -28923,11 +29327,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="87"/>
       <c r="L40" s="78"/>
-      <c r="M40" s="355">
+      <c r="M40" s="356">
         <f>SUM(M5:M39)</f>
         <v>1636108</v>
       </c>
-      <c r="N40" s="339">
+      <c r="N40" s="340">
         <f>SUM(N5:N39)</f>
         <v>55675</v>
       </c>
@@ -28952,8 +29356,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="74"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="338"/>
-      <c r="N41" s="340"/>
+      <c r="M41" s="339"/>
+      <c r="N41" s="341"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -29160,29 +29564,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="341" t="s">
+      <c r="H53" s="342" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="342"/>
+      <c r="I53" s="343"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="343">
+      <c r="K53" s="344">
         <f>I51+L51</f>
         <v>45634.280000000006</v>
       </c>
-      <c r="L53" s="344"/>
-      <c r="M53" s="345">
+      <c r="L53" s="345"/>
+      <c r="M53" s="346">
         <f>N40+M40</f>
         <v>1691783</v>
       </c>
-      <c r="N53" s="346"/>
+      <c r="N53" s="347"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="347" t="s">
+      <c r="D54" s="348" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="347"/>
+      <c r="E54" s="348"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>1686442.72</v>
@@ -29193,22 +29597,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="348" t="s">
+      <c r="D55" s="349" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="348"/>
+      <c r="E55" s="349"/>
       <c r="F55" s="111">
         <v>-1631962.77</v>
       </c>
-      <c r="I55" s="349" t="s">
+      <c r="I55" s="350" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="350"/>
-      <c r="K55" s="351">
+      <c r="J55" s="351"/>
+      <c r="K55" s="352">
         <f>F57+F58+F59</f>
         <v>238822.13999999996</v>
       </c>
-      <c r="L55" s="352"/>
+      <c r="L55" s="353"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -29239,11 +29643,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="353">
+      <c r="K57" s="354">
         <f>-C4</f>
         <v>-154314.51999999999</v>
       </c>
-      <c r="L57" s="354"/>
+      <c r="L57" s="355"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -29260,22 +29664,22 @@
       <c r="C59" s="128">
         <v>44619</v>
       </c>
-      <c r="D59" s="330" t="s">
+      <c r="D59" s="331" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="331"/>
+      <c r="E59" s="332"/>
       <c r="F59" s="129">
         <v>184342.19</v>
       </c>
-      <c r="I59" s="332" t="s">
+      <c r="I59" s="333" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="333"/>
-      <c r="K59" s="334">
+      <c r="J59" s="334"/>
+      <c r="K59" s="335">
         <f>K55+K57</f>
         <v>84507.619999999966</v>
       </c>
-      <c r="L59" s="334"/>
+      <c r="L59" s="335"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -30725,23 +31129,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="317"/>
-      <c r="C1" s="319" t="s">
+      <c r="B1" s="318"/>
+      <c r="C1" s="320" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="320"/>
-      <c r="E1" s="320"/>
-      <c r="F1" s="320"/>
-      <c r="G1" s="320"/>
-      <c r="H1" s="320"/>
-      <c r="I1" s="320"/>
-      <c r="J1" s="320"/>
-      <c r="K1" s="320"/>
-      <c r="L1" s="320"/>
-      <c r="M1" s="320"/>
+      <c r="D1" s="321"/>
+      <c r="E1" s="321"/>
+      <c r="F1" s="321"/>
+      <c r="G1" s="321"/>
+      <c r="H1" s="321"/>
+      <c r="I1" s="321"/>
+      <c r="J1" s="321"/>
+      <c r="K1" s="321"/>
+      <c r="L1" s="321"/>
+      <c r="M1" s="321"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="318"/>
+      <c r="B2" s="319"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -30751,21 +31155,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="321" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="322"/>
+      <c r="B3" s="322" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="323"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="323" t="s">
+      <c r="H3" s="324" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="323"/>
+      <c r="I3" s="324"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="328" t="s">
+      <c r="R3" s="329" t="s">
         <v>38</v>
       </c>
     </row>
@@ -30780,14 +31184,14 @@
       <c r="D4" s="16">
         <v>44619</v>
       </c>
-      <c r="E4" s="324" t="s">
+      <c r="E4" s="325" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="325"/>
-      <c r="H4" s="326" t="s">
+      <c r="F4" s="326"/>
+      <c r="H4" s="327" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="327"/>
+      <c r="I4" s="328"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -30797,11 +31201,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="335" t="s">
+      <c r="P4" s="336" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="336"/>
-      <c r="R4" s="329"/>
+      <c r="Q4" s="337"/>
+      <c r="R4" s="330"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -32252,11 +32656,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="87"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="337">
+      <c r="M40" s="338">
         <f>SUM(M5:M39)</f>
         <v>1793435</v>
       </c>
-      <c r="N40" s="339">
+      <c r="N40" s="340">
         <f>SUM(N5:N39)</f>
         <v>63995</v>
       </c>
@@ -32281,8 +32685,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="235"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="338"/>
-      <c r="N41" s="340"/>
+      <c r="M41" s="339"/>
+      <c r="N41" s="341"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -32421,29 +32825,29 @@
       <c r="A49" s="33"/>
       <c r="B49" s="113"/>
       <c r="C49" s="1"/>
-      <c r="H49" s="341" t="s">
+      <c r="H49" s="342" t="s">
         <v>12</v>
       </c>
-      <c r="I49" s="342"/>
+      <c r="I49" s="343"/>
       <c r="J49" s="114"/>
-      <c r="K49" s="343">
+      <c r="K49" s="344">
         <f>I47+L47</f>
         <v>90434.03</v>
       </c>
-      <c r="L49" s="344"/>
-      <c r="M49" s="345">
+      <c r="L49" s="345"/>
+      <c r="M49" s="346">
         <f>N40+M40</f>
         <v>1857430</v>
       </c>
-      <c r="N49" s="346"/>
+      <c r="N49" s="347"/>
       <c r="P49" s="32"/>
       <c r="Q49" s="8"/>
     </row>
     <row r="50" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D50" s="347" t="s">
+      <c r="D50" s="348" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="347"/>
+      <c r="E50" s="348"/>
       <c r="F50" s="115">
         <f>F47-K49-C47</f>
         <v>1824260.97</v>
@@ -32454,22 +32858,22 @@
       <c r="Q50" s="8"/>
     </row>
     <row r="51" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D51" s="348" t="s">
+      <c r="D51" s="349" t="s">
         <v>14</v>
       </c>
-      <c r="E51" s="348"/>
+      <c r="E51" s="349"/>
       <c r="F51" s="111">
         <v>-1848136.64</v>
       </c>
-      <c r="I51" s="349" t="s">
+      <c r="I51" s="350" t="s">
         <v>15</v>
       </c>
-      <c r="J51" s="350"/>
-      <c r="K51" s="351">
+      <c r="J51" s="351"/>
+      <c r="K51" s="352">
         <f>F53+F54+F55</f>
         <v>195541.70000000007</v>
       </c>
-      <c r="L51" s="352"/>
+      <c r="L51" s="353"/>
       <c r="P51" s="32"/>
       <c r="Q51" s="8"/>
     </row>
@@ -32500,11 +32904,11 @@
         <v>17</v>
       </c>
       <c r="J53" s="125"/>
-      <c r="K53" s="353">
+      <c r="K53" s="354">
         <f>-C4</f>
         <v>-184342.19</v>
       </c>
-      <c r="L53" s="354"/>
+      <c r="L53" s="355"/>
     </row>
     <row r="54" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D54" s="126" t="s">
@@ -32521,22 +32925,22 @@
       <c r="C55" s="128">
         <v>44647</v>
       </c>
-      <c r="D55" s="330" t="s">
+      <c r="D55" s="331" t="s">
         <v>20</v>
       </c>
-      <c r="E55" s="331"/>
+      <c r="E55" s="332"/>
       <c r="F55" s="129">
         <v>219417.37</v>
       </c>
-      <c r="I55" s="332" t="s">
+      <c r="I55" s="333" t="s">
         <v>226</v>
       </c>
-      <c r="J55" s="333"/>
-      <c r="K55" s="334">
+      <c r="J55" s="334"/>
+      <c r="K55" s="335">
         <f>K51+K53</f>
         <v>11199.510000000068</v>
       </c>
-      <c r="L55" s="334"/>
+      <c r="L55" s="335"/>
     </row>
     <row r="56" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C56" s="130"/>
@@ -34159,23 +34563,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="317"/>
-      <c r="C1" s="319" t="s">
+      <c r="B1" s="318"/>
+      <c r="C1" s="320" t="s">
         <v>225</v>
       </c>
-      <c r="D1" s="320"/>
-      <c r="E1" s="320"/>
-      <c r="F1" s="320"/>
-      <c r="G1" s="320"/>
-      <c r="H1" s="320"/>
-      <c r="I1" s="320"/>
-      <c r="J1" s="320"/>
-      <c r="K1" s="320"/>
-      <c r="L1" s="320"/>
-      <c r="M1" s="320"/>
+      <c r="D1" s="321"/>
+      <c r="E1" s="321"/>
+      <c r="F1" s="321"/>
+      <c r="G1" s="321"/>
+      <c r="H1" s="321"/>
+      <c r="I1" s="321"/>
+      <c r="J1" s="321"/>
+      <c r="K1" s="321"/>
+      <c r="L1" s="321"/>
+      <c r="M1" s="321"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="318"/>
+      <c r="B2" s="319"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -34185,21 +34589,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="321" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="322"/>
+      <c r="B3" s="322" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="323"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="323" t="s">
+      <c r="H3" s="324" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="323"/>
+      <c r="I3" s="324"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="328" t="s">
+      <c r="R3" s="329" t="s">
         <v>38</v>
       </c>
     </row>
@@ -34214,14 +34618,14 @@
       <c r="D4" s="16">
         <v>44647</v>
       </c>
-      <c r="E4" s="324" t="s">
+      <c r="E4" s="325" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="325"/>
-      <c r="H4" s="326" t="s">
+      <c r="F4" s="326"/>
+      <c r="H4" s="327" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="327"/>
+      <c r="I4" s="328"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -34231,11 +34635,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="335" t="s">
+      <c r="P4" s="336" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="336"/>
-      <c r="R4" s="329"/>
+      <c r="Q4" s="337"/>
+      <c r="R4" s="330"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -35832,11 +36236,11 @@
         <f>927.48+128</f>
         <v>1055.48</v>
       </c>
-      <c r="M40" s="337">
+      <c r="M40" s="338">
         <f>SUM(M5:M39)</f>
         <v>2146671</v>
       </c>
-      <c r="N40" s="339">
+      <c r="N40" s="340">
         <f>SUM(N5:N39)</f>
         <v>68590</v>
       </c>
@@ -35867,8 +36271,8 @@
       <c r="L41" s="73">
         <v>1195.68</v>
       </c>
-      <c r="M41" s="338"/>
-      <c r="N41" s="340"/>
+      <c r="M41" s="339"/>
+      <c r="N41" s="341"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -36099,29 +36503,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="341" t="s">
+      <c r="H53" s="342" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="342"/>
+      <c r="I53" s="343"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="343">
+      <c r="K53" s="344">
         <f>I51+L51</f>
         <v>91272.77</v>
       </c>
-      <c r="L53" s="344"/>
-      <c r="M53" s="345">
+      <c r="L53" s="345"/>
+      <c r="M53" s="346">
         <f>N40+M40</f>
         <v>2215261</v>
       </c>
-      <c r="N53" s="346"/>
+      <c r="N53" s="347"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="347" t="s">
+      <c r="D54" s="348" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="347"/>
+      <c r="E54" s="348"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2179879.23</v>
@@ -36132,22 +36536,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="348" t="s">
+      <c r="D55" s="349" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="348"/>
+      <c r="E55" s="349"/>
       <c r="F55" s="111">
         <v>-2227493.48</v>
       </c>
-      <c r="I55" s="349" t="s">
+      <c r="I55" s="350" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="350"/>
-      <c r="K55" s="351">
+      <c r="J55" s="351"/>
+      <c r="K55" s="352">
         <f>F57+F58+F59</f>
         <v>261521.34000000003</v>
       </c>
-      <c r="L55" s="352"/>
+      <c r="L55" s="353"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -36178,11 +36582,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="353">
+      <c r="K57" s="354">
         <f>-C4</f>
         <v>-219417.37</v>
       </c>
-      <c r="L57" s="354"/>
+      <c r="L57" s="355"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -36199,22 +36603,22 @@
       <c r="C59" s="128">
         <v>44682</v>
       </c>
-      <c r="D59" s="330" t="s">
+      <c r="D59" s="331" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="331"/>
+      <c r="E59" s="332"/>
       <c r="F59" s="129">
         <v>297874.59000000003</v>
       </c>
-      <c r="I59" s="332" t="s">
+      <c r="I59" s="333" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="333"/>
-      <c r="K59" s="334">
+      <c r="J59" s="334"/>
+      <c r="K59" s="335">
         <f>K55+K57</f>
         <v>42103.97000000003</v>
       </c>
-      <c r="L59" s="334"/>
+      <c r="L59" s="335"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>
@@ -37866,23 +38270,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="317"/>
-      <c r="C1" s="319" t="s">
+      <c r="B1" s="318"/>
+      <c r="C1" s="320" t="s">
         <v>277</v>
       </c>
-      <c r="D1" s="320"/>
-      <c r="E1" s="320"/>
-      <c r="F1" s="320"/>
-      <c r="G1" s="320"/>
-      <c r="H1" s="320"/>
-      <c r="I1" s="320"/>
-      <c r="J1" s="320"/>
-      <c r="K1" s="320"/>
-      <c r="L1" s="320"/>
-      <c r="M1" s="320"/>
+      <c r="D1" s="321"/>
+      <c r="E1" s="321"/>
+      <c r="F1" s="321"/>
+      <c r="G1" s="321"/>
+      <c r="H1" s="321"/>
+      <c r="I1" s="321"/>
+      <c r="J1" s="321"/>
+      <c r="K1" s="321"/>
+      <c r="L1" s="321"/>
+      <c r="M1" s="321"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="318"/>
+      <c r="B2" s="319"/>
       <c r="C2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -37892,21 +38296,21 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="321" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="322"/>
+      <c r="B3" s="322" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="323"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="323" t="s">
+      <c r="H3" s="324" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="323"/>
+      <c r="I3" s="324"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="4"/>
-      <c r="R3" s="328" t="s">
+      <c r="R3" s="329" t="s">
         <v>38</v>
       </c>
     </row>
@@ -37921,14 +38325,14 @@
       <c r="D4" s="16">
         <v>44682</v>
       </c>
-      <c r="E4" s="324" t="s">
+      <c r="E4" s="325" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="325"/>
-      <c r="H4" s="326" t="s">
+      <c r="F4" s="326"/>
+      <c r="H4" s="327" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="327"/>
+      <c r="I4" s="328"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -37938,11 +38342,11 @@
       <c r="N4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="335" t="s">
+      <c r="P4" s="336" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="336"/>
-      <c r="R4" s="329"/>
+      <c r="Q4" s="337"/>
+      <c r="R4" s="330"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -39459,11 +39863,11 @@
       <c r="J40" s="71"/>
       <c r="K40" s="74"/>
       <c r="L40" s="73"/>
-      <c r="M40" s="337">
+      <c r="M40" s="338">
         <f>SUM(M5:M39)</f>
         <v>2144215</v>
       </c>
-      <c r="N40" s="339">
+      <c r="N40" s="340">
         <f>SUM(N5:N39)</f>
         <v>62525</v>
       </c>
@@ -39488,8 +39892,8 @@
       <c r="J41" s="71"/>
       <c r="K41" s="235"/>
       <c r="L41" s="73"/>
-      <c r="M41" s="338"/>
-      <c r="N41" s="340"/>
+      <c r="M41" s="339"/>
+      <c r="N41" s="341"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="8"/>
     </row>
@@ -39700,29 +40104,29 @@
       <c r="A53" s="33"/>
       <c r="B53" s="113"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="341" t="s">
+      <c r="H53" s="342" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="342"/>
+      <c r="I53" s="343"/>
       <c r="J53" s="114"/>
-      <c r="K53" s="343">
+      <c r="K53" s="344">
         <f>I51+L51</f>
         <v>51231.42</v>
       </c>
-      <c r="L53" s="344"/>
-      <c r="M53" s="345">
+      <c r="L53" s="345"/>
+      <c r="M53" s="346">
         <f>N40+M40</f>
         <v>2206740</v>
       </c>
-      <c r="N53" s="346"/>
+      <c r="N53" s="347"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="347" t="s">
+      <c r="D54" s="348" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="347"/>
+      <c r="E54" s="348"/>
       <c r="F54" s="115">
         <f>F51-K53-C51</f>
         <v>2189405.58</v>
@@ -39733,22 +40137,22 @@
       <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="348" t="s">
+      <c r="D55" s="349" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="348"/>
+      <c r="E55" s="349"/>
       <c r="F55" s="111">
         <v>-2251924.65</v>
       </c>
-      <c r="I55" s="349" t="s">
+      <c r="I55" s="350" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="350"/>
-      <c r="K55" s="351">
+      <c r="J55" s="351"/>
+      <c r="K55" s="352">
         <f>F57+F58+F59</f>
         <v>112552.74000000017</v>
       </c>
-      <c r="L55" s="352"/>
+      <c r="L55" s="353"/>
       <c r="P55" s="32"/>
       <c r="Q55" s="8"/>
     </row>
@@ -39779,11 +40183,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="125"/>
-      <c r="K57" s="353">
+      <c r="K57" s="354">
         <f>-C4</f>
         <v>-297874.59000000003</v>
       </c>
-      <c r="L57" s="354"/>
+      <c r="L57" s="355"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="126" t="s">
@@ -39800,22 +40204,22 @@
       <c r="C59" s="128">
         <v>44710</v>
       </c>
-      <c r="D59" s="330" t="s">
+      <c r="D59" s="331" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="331"/>
+      <c r="E59" s="332"/>
       <c r="F59" s="129">
         <v>149938.81</v>
       </c>
-      <c r="I59" s="332" t="s">
+      <c r="I59" s="333" t="s">
         <v>325</v>
       </c>
-      <c r="J59" s="333"/>
-      <c r="K59" s="334">
+      <c r="J59" s="334"/>
+      <c r="K59" s="335">
         <f>K55+K57</f>
         <v>-185321.84999999986</v>
       </c>
-      <c r="L59" s="334"/>
+      <c r="L59" s="335"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="130"/>

</xml_diff>